<commit_message>
updated creating plot for china
</commit_message>
<xml_diff>
--- a/COVID19-Confirmed.xlsx
+++ b/COVID19-Confirmed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="128">
   <si>
     <t>Province/State</t>
   </si>
@@ -154,6 +154,15 @@
     <t>2/12/20 22:00</t>
   </si>
   <si>
+    <t>2/13/20 10:00</t>
+  </si>
+  <si>
+    <t>2/13/20 21:15</t>
+  </si>
+  <si>
+    <t>2/14/20 11:23</t>
+  </si>
+  <si>
     <t>Anhui</t>
   </si>
   <si>
@@ -308,6 +317,9 @@
   </si>
   <si>
     <t>San Diego County, CA</t>
+  </si>
+  <si>
+    <t>San Antonio, TX</t>
   </si>
   <si>
     <t>Mainland China</t>
@@ -743,13 +755,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AT74"/>
+  <dimension ref="A1:AW75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:46">
+    <row r="1" spans="1:49">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -888,13 +900,22 @@
       <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="AU1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="2" spans="1:46">
+    <row r="2" spans="1:49">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C2">
         <v>31.82571</v>
@@ -1028,13 +1049,22 @@
       <c r="AT2">
         <v>910</v>
       </c>
+      <c r="AU2">
+        <v>910</v>
+      </c>
+      <c r="AV2">
+        <v>934</v>
+      </c>
+      <c r="AW2">
+        <v>934</v>
+      </c>
     </row>
-    <row r="3" spans="1:46">
+    <row r="3" spans="1:49">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C3">
         <v>40.18238</v>
@@ -1168,13 +1198,22 @@
       <c r="AT3">
         <v>366</v>
       </c>
+      <c r="AU3">
+        <v>366</v>
+      </c>
+      <c r="AV3">
+        <v>366</v>
+      </c>
+      <c r="AW3">
+        <v>372</v>
+      </c>
     </row>
-    <row r="4" spans="1:46">
+    <row r="4" spans="1:49">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C4">
         <v>30.05718</v>
@@ -1308,13 +1347,22 @@
       <c r="AT4">
         <v>518</v>
       </c>
+      <c r="AU4">
+        <v>525</v>
+      </c>
+      <c r="AV4">
+        <v>529</v>
+      </c>
+      <c r="AW4">
+        <v>532</v>
+      </c>
     </row>
-    <row r="5" spans="1:46">
+    <row r="5" spans="1:49">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C5">
         <v>26.07783</v>
@@ -1448,13 +1496,22 @@
       <c r="AT5">
         <v>279</v>
       </c>
+      <c r="AU5">
+        <v>279</v>
+      </c>
+      <c r="AV5">
+        <v>281</v>
+      </c>
+      <c r="AW5">
+        <v>281</v>
+      </c>
     </row>
-    <row r="6" spans="1:46">
+    <row r="6" spans="1:49">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C6">
         <v>36.0611</v>
@@ -1588,13 +1645,22 @@
       <c r="AT6">
         <v>87</v>
       </c>
+      <c r="AU6">
+        <v>87</v>
+      </c>
+      <c r="AV6">
+        <v>90</v>
+      </c>
+      <c r="AW6">
+        <v>90</v>
+      </c>
     </row>
-    <row r="7" spans="1:46">
+    <row r="7" spans="1:49">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C7">
         <v>23.33841</v>
@@ -1728,13 +1794,22 @@
       <c r="AT7">
         <v>1241</v>
       </c>
+      <c r="AU7">
+        <v>1241</v>
+      </c>
+      <c r="AV7">
+        <v>1261</v>
+      </c>
+      <c r="AW7">
+        <v>1261</v>
+      </c>
     </row>
-    <row r="8" spans="1:46">
+    <row r="8" spans="1:49">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C8">
         <v>23.82908</v>
@@ -1868,13 +1943,22 @@
       <c r="AT8">
         <v>222</v>
       </c>
+      <c r="AU8">
+        <v>222</v>
+      </c>
+      <c r="AV8">
+        <v>226</v>
+      </c>
+      <c r="AW8">
+        <v>226</v>
+      </c>
     </row>
-    <row r="9" spans="1:46">
+    <row r="9" spans="1:49">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C9">
         <v>26.81536</v>
@@ -2008,13 +2092,22 @@
       <c r="AT9">
         <v>135</v>
       </c>
+      <c r="AU9">
+        <v>135</v>
+      </c>
+      <c r="AV9">
+        <v>140</v>
+      </c>
+      <c r="AW9">
+        <v>140</v>
+      </c>
     </row>
-    <row r="10" spans="1:46">
+    <row r="10" spans="1:49">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C10">
         <v>19.19673</v>
@@ -2148,13 +2241,22 @@
       <c r="AT10">
         <v>157</v>
       </c>
+      <c r="AU10">
+        <v>157</v>
+      </c>
+      <c r="AV10">
+        <v>158</v>
+      </c>
+      <c r="AW10">
+        <v>159</v>
+      </c>
     </row>
-    <row r="11" spans="1:46">
+    <row r="11" spans="1:49">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C11">
         <v>38.0428</v>
@@ -2288,13 +2390,22 @@
       <c r="AT11">
         <v>265</v>
       </c>
+      <c r="AU11">
+        <v>265</v>
+      </c>
+      <c r="AV11">
+        <v>283</v>
+      </c>
+      <c r="AW11">
+        <v>283</v>
+      </c>
     </row>
-    <row r="12" spans="1:46">
+    <row r="12" spans="1:49">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C12">
         <v>47.862</v>
@@ -2428,13 +2539,22 @@
       <c r="AT12">
         <v>395</v>
       </c>
+      <c r="AU12">
+        <v>395</v>
+      </c>
+      <c r="AV12">
+        <v>418</v>
+      </c>
+      <c r="AW12">
+        <v>419</v>
+      </c>
     </row>
-    <row r="13" spans="1:46">
+    <row r="13" spans="1:49">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C13">
         <v>33.88202</v>
@@ -2568,13 +2688,22 @@
       <c r="AT13">
         <v>1169</v>
       </c>
+      <c r="AU13">
+        <v>1169</v>
+      </c>
+      <c r="AV13">
+        <v>1184</v>
+      </c>
+      <c r="AW13">
+        <v>1184</v>
+      </c>
     </row>
-    <row r="14" spans="1:46">
+    <row r="14" spans="1:49">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C14">
         <v>30.97564</v>
@@ -2708,13 +2837,22 @@
       <c r="AT14">
         <v>48206</v>
       </c>
+      <c r="AU14">
+        <v>48206</v>
+      </c>
+      <c r="AV14">
+        <v>51986</v>
+      </c>
+      <c r="AW14">
+        <v>51986</v>
+      </c>
     </row>
-    <row r="15" spans="1:46">
+    <row r="15" spans="1:49">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C15">
         <v>27.61041</v>
@@ -2848,13 +2986,22 @@
       <c r="AT15">
         <v>968</v>
       </c>
+      <c r="AU15">
+        <v>968</v>
+      </c>
+      <c r="AV15">
+        <v>988</v>
+      </c>
+      <c r="AW15">
+        <v>988</v>
+      </c>
     </row>
-    <row r="16" spans="1:46">
+    <row r="16" spans="1:49">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C16">
         <v>44.09448</v>
@@ -2988,13 +3135,22 @@
       <c r="AT16">
         <v>61</v>
       </c>
+      <c r="AU16">
+        <v>61</v>
+      </c>
+      <c r="AV16">
+        <v>65</v>
+      </c>
+      <c r="AW16">
+        <v>65</v>
+      </c>
     </row>
-    <row r="17" spans="1:46">
+    <row r="17" spans="1:49">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C17">
         <v>32.97027</v>
@@ -3128,13 +3284,22 @@
       <c r="AT17">
         <v>570</v>
       </c>
+      <c r="AU17">
+        <v>570</v>
+      </c>
+      <c r="AV17">
+        <v>593</v>
+      </c>
+      <c r="AW17">
+        <v>593</v>
+      </c>
     </row>
-    <row r="18" spans="1:46">
+    <row r="18" spans="1:49">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C18">
         <v>27.61401</v>
@@ -3268,13 +3433,22 @@
       <c r="AT18">
         <v>872</v>
       </c>
+      <c r="AU18">
+        <v>872</v>
+      </c>
+      <c r="AV18">
+        <v>900</v>
+      </c>
+      <c r="AW18">
+        <v>900</v>
+      </c>
     </row>
-    <row r="19" spans="1:46">
+    <row r="19" spans="1:49">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C19">
         <v>43.66657</v>
@@ -3408,13 +3582,22 @@
       <c r="AT19">
         <v>84</v>
       </c>
+      <c r="AU19">
+        <v>84</v>
+      </c>
+      <c r="AV19">
+        <v>86</v>
+      </c>
+      <c r="AW19">
+        <v>86</v>
+      </c>
     </row>
-    <row r="20" spans="1:46">
+    <row r="20" spans="1:49">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C20">
         <v>41.29284000000001</v>
@@ -3548,13 +3731,22 @@
       <c r="AT20">
         <v>116</v>
       </c>
+      <c r="AU20">
+        <v>117</v>
+      </c>
+      <c r="AV20">
+        <v>117</v>
+      </c>
+      <c r="AW20">
+        <v>119</v>
+      </c>
     </row>
-    <row r="21" spans="1:46">
+    <row r="21" spans="1:49">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C21">
         <v>37.26923</v>
@@ -3688,13 +3880,22 @@
       <c r="AT21">
         <v>64</v>
       </c>
+      <c r="AU21">
+        <v>64</v>
+      </c>
+      <c r="AV21">
+        <v>67</v>
+      </c>
+      <c r="AW21">
+        <v>67</v>
+      </c>
     </row>
-    <row r="22" spans="1:46">
+    <row r="22" spans="1:49">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C22">
         <v>35.65945</v>
@@ -3828,13 +4029,22 @@
       <c r="AT22">
         <v>18</v>
       </c>
+      <c r="AU22">
+        <v>18</v>
+      </c>
+      <c r="AV22">
+        <v>18</v>
+      </c>
+      <c r="AW22">
+        <v>18</v>
+      </c>
     </row>
-    <row r="23" spans="1:46">
+    <row r="23" spans="1:49">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C23">
         <v>35.19165</v>
@@ -3968,13 +4178,22 @@
       <c r="AT23">
         <v>229</v>
       </c>
+      <c r="AU23">
+        <v>229</v>
+      </c>
+      <c r="AV23">
+        <v>229</v>
+      </c>
+      <c r="AW23">
+        <v>230</v>
+      </c>
     </row>
-    <row r="24" spans="1:46">
+    <row r="24" spans="1:49">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C24">
         <v>36.34377</v>
@@ -4108,13 +4327,22 @@
       <c r="AT24">
         <v>506</v>
       </c>
+      <c r="AU24">
+        <v>509</v>
+      </c>
+      <c r="AV24">
+        <v>519</v>
+      </c>
+      <c r="AW24">
+        <v>523</v>
+      </c>
     </row>
-    <row r="25" spans="1:46">
+    <row r="25" spans="1:49">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C25">
         <v>31.20327</v>
@@ -4248,13 +4476,22 @@
       <c r="AT25">
         <v>313</v>
       </c>
+      <c r="AU25">
+        <v>315</v>
+      </c>
+      <c r="AV25">
+        <v>318</v>
+      </c>
+      <c r="AW25">
+        <v>318</v>
+      </c>
     </row>
-    <row r="26" spans="1:46">
+    <row r="26" spans="1:49">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C26">
         <v>37.57769</v>
@@ -4388,13 +4625,22 @@
       <c r="AT26">
         <v>126</v>
       </c>
+      <c r="AU26">
+        <v>126</v>
+      </c>
+      <c r="AV26">
+        <v>126</v>
+      </c>
+      <c r="AW26">
+        <v>126</v>
+      </c>
     </row>
-    <row r="27" spans="1:46">
+    <row r="27" spans="1:49">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C27">
         <v>30.61714000000001</v>
@@ -4528,13 +4774,22 @@
       <c r="AT27">
         <v>451</v>
       </c>
+      <c r="AU27">
+        <v>451</v>
+      </c>
+      <c r="AV27">
+        <v>463</v>
+      </c>
+      <c r="AW27">
+        <v>463</v>
+      </c>
     </row>
-    <row r="28" spans="1:46">
+    <row r="28" spans="1:49">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C28">
         <v>39.29362</v>
@@ -4668,13 +4923,22 @@
       <c r="AT28">
         <v>113</v>
       </c>
+      <c r="AU28">
+        <v>117</v>
+      </c>
+      <c r="AV28">
+        <v>119</v>
+      </c>
+      <c r="AW28">
+        <v>120</v>
+      </c>
     </row>
-    <row r="29" spans="1:46">
+    <row r="29" spans="1:49">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C29">
         <v>30.1534</v>
@@ -4808,13 +5072,22 @@
       <c r="AT29">
         <v>1</v>
       </c>
+      <c r="AU29">
+        <v>1</v>
+      </c>
+      <c r="AV29">
+        <v>1</v>
+      </c>
+      <c r="AW29">
+        <v>1</v>
+      </c>
     </row>
-    <row r="30" spans="1:46">
+    <row r="30" spans="1:49">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C30">
         <v>41.11981</v>
@@ -4948,13 +5221,22 @@
       <c r="AT30">
         <v>63</v>
       </c>
+      <c r="AU30">
+        <v>63</v>
+      </c>
+      <c r="AV30">
+        <v>65</v>
+      </c>
+      <c r="AW30">
+        <v>65</v>
+      </c>
     </row>
-    <row r="31" spans="1:46">
+    <row r="31" spans="1:49">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C31">
         <v>24.97411</v>
@@ -5088,13 +5370,22 @@
       <c r="AT31">
         <v>155</v>
       </c>
+      <c r="AU31">
+        <v>156</v>
+      </c>
+      <c r="AV31">
+        <v>156</v>
+      </c>
+      <c r="AW31">
+        <v>162</v>
+      </c>
     </row>
-    <row r="32" spans="1:46">
+    <row r="32" spans="1:49">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C32">
         <v>29.18251</v>
@@ -5228,10 +5519,19 @@
       <c r="AT32">
         <v>1145</v>
       </c>
+      <c r="AU32">
+        <v>1145</v>
+      </c>
+      <c r="AV32">
+        <v>1155</v>
+      </c>
+      <c r="AW32">
+        <v>1155</v>
+      </c>
     </row>
-    <row r="33" spans="1:46">
+    <row r="33" spans="1:49">
       <c r="B33" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C33">
         <v>13.7563</v>
@@ -5365,10 +5665,19 @@
       <c r="AT33">
         <v>33</v>
       </c>
+      <c r="AU33">
+        <v>33</v>
+      </c>
+      <c r="AV33">
+        <v>33</v>
+      </c>
+      <c r="AW33">
+        <v>33</v>
+      </c>
     </row>
-    <row r="34" spans="1:46">
+    <row r="34" spans="1:49">
       <c r="B34" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C34">
         <v>35.6762</v>
@@ -5502,10 +5811,19 @@
       <c r="AT34">
         <v>28</v>
       </c>
+      <c r="AU34">
+        <v>28</v>
+      </c>
+      <c r="AV34">
+        <v>28</v>
+      </c>
+      <c r="AW34">
+        <v>29</v>
+      </c>
     </row>
-    <row r="35" spans="1:46">
+    <row r="35" spans="1:49">
       <c r="B35" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C35">
         <v>37.5665</v>
@@ -5639,13 +5957,22 @@
       <c r="AT35">
         <v>28</v>
       </c>
+      <c r="AU35">
+        <v>28</v>
+      </c>
+      <c r="AV35">
+        <v>28</v>
+      </c>
+      <c r="AW35">
+        <v>28</v>
+      </c>
     </row>
-    <row r="36" spans="1:46">
+    <row r="36" spans="1:49">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C36">
         <v>23.6978</v>
@@ -5779,13 +6106,22 @@
       <c r="AT36">
         <v>18</v>
       </c>
+      <c r="AU36">
+        <v>18</v>
+      </c>
+      <c r="AV36">
+        <v>18</v>
+      </c>
+      <c r="AW36">
+        <v>18</v>
+      </c>
     </row>
-    <row r="37" spans="1:46">
+    <row r="37" spans="1:49">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C37">
         <v>47.7511</v>
@@ -5919,13 +6255,22 @@
       <c r="AT37">
         <v>1</v>
       </c>
+      <c r="AU37">
+        <v>1</v>
+      </c>
+      <c r="AV37">
+        <v>1</v>
+      </c>
+      <c r="AW37">
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="1:46">
+    <row r="38" spans="1:49">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C38">
         <v>40.6331</v>
@@ -6059,13 +6404,22 @@
       <c r="AT38">
         <v>2</v>
       </c>
+      <c r="AU38">
+        <v>2</v>
+      </c>
+      <c r="AV38">
+        <v>2</v>
+      </c>
+      <c r="AW38">
+        <v>2</v>
+      </c>
     </row>
-    <row r="39" spans="1:46">
+    <row r="39" spans="1:49">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C39">
         <v>34.0489</v>
@@ -6199,13 +6553,22 @@
       <c r="AT39">
         <v>1</v>
       </c>
+      <c r="AU39">
+        <v>1</v>
+      </c>
+      <c r="AV39">
+        <v>1</v>
+      </c>
+      <c r="AW39">
+        <v>1</v>
+      </c>
     </row>
-    <row r="40" spans="1:46">
+    <row r="40" spans="1:49">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C40">
         <v>22.1987</v>
@@ -6339,13 +6702,22 @@
       <c r="AT40">
         <v>10</v>
       </c>
+      <c r="AU40">
+        <v>10</v>
+      </c>
+      <c r="AV40">
+        <v>10</v>
+      </c>
+      <c r="AW40">
+        <v>10</v>
+      </c>
     </row>
-    <row r="41" spans="1:46">
+    <row r="41" spans="1:49">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C41">
         <v>22.3193</v>
@@ -6479,10 +6851,19 @@
       <c r="AT41">
         <v>50</v>
       </c>
+      <c r="AU41">
+        <v>53</v>
+      </c>
+      <c r="AV41">
+        <v>53</v>
+      </c>
+      <c r="AW41">
+        <v>56</v>
+      </c>
     </row>
-    <row r="42" spans="1:46">
+    <row r="42" spans="1:49">
       <c r="B42" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C42">
         <v>1.3521</v>
@@ -6616,10 +6997,19 @@
       <c r="AT42">
         <v>50</v>
       </c>
+      <c r="AU42">
+        <v>58</v>
+      </c>
+      <c r="AV42">
+        <v>58</v>
+      </c>
+      <c r="AW42">
+        <v>67</v>
+      </c>
     </row>
-    <row r="43" spans="1:46">
+    <row r="43" spans="1:49">
       <c r="B43" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C43">
         <v>21.0278</v>
@@ -6753,10 +7143,19 @@
       <c r="AT43">
         <v>15</v>
       </c>
+      <c r="AU43">
+        <v>16</v>
+      </c>
+      <c r="AV43">
+        <v>16</v>
+      </c>
+      <c r="AW43">
+        <v>16</v>
+      </c>
     </row>
-    <row r="44" spans="1:46">
+    <row r="44" spans="1:49">
       <c r="B44" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C44">
         <v>46.2276</v>
@@ -6890,10 +7289,19 @@
       <c r="AT44">
         <v>11</v>
       </c>
+      <c r="AU44">
+        <v>11</v>
+      </c>
+      <c r="AV44">
+        <v>11</v>
+      </c>
+      <c r="AW44">
+        <v>11</v>
+      </c>
     </row>
-    <row r="45" spans="1:46">
+    <row r="45" spans="1:49">
       <c r="B45" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C45">
         <v>28.3949</v>
@@ -7027,10 +7435,19 @@
       <c r="AT45">
         <v>1</v>
       </c>
+      <c r="AU45">
+        <v>1</v>
+      </c>
+      <c r="AV45">
+        <v>1</v>
+      </c>
+      <c r="AW45">
+        <v>1</v>
+      </c>
     </row>
-    <row r="46" spans="1:46">
+    <row r="46" spans="1:49">
       <c r="B46" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C46">
         <v>4.2105</v>
@@ -7164,13 +7581,22 @@
       <c r="AT46">
         <v>18</v>
       </c>
+      <c r="AU46">
+        <v>19</v>
+      </c>
+      <c r="AV46">
+        <v>19</v>
+      </c>
+      <c r="AW46">
+        <v>19</v>
+      </c>
     </row>
-    <row r="47" spans="1:46">
+    <row r="47" spans="1:49">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B47" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C47">
         <v>43.6532</v>
@@ -7304,13 +7730,22 @@
       <c r="AT47">
         <v>2</v>
       </c>
+      <c r="AU47">
+        <v>2</v>
+      </c>
+      <c r="AV47">
+        <v>2</v>
+      </c>
+      <c r="AW47">
+        <v>2</v>
+      </c>
     </row>
-    <row r="48" spans="1:46">
+    <row r="48" spans="1:49">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C48">
         <v>49.2827</v>
@@ -7444,13 +7879,22 @@
       <c r="AT48">
         <v>4</v>
       </c>
+      <c r="AU48">
+        <v>4</v>
+      </c>
+      <c r="AV48">
+        <v>4</v>
+      </c>
+      <c r="AW48">
+        <v>4</v>
+      </c>
     </row>
-    <row r="49" spans="1:46">
+    <row r="49" spans="1:49">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C49">
         <v>33.7879</v>
@@ -7584,13 +8028,22 @@
       <c r="AT49">
         <v>1</v>
       </c>
+      <c r="AU49">
+        <v>1</v>
+      </c>
+      <c r="AV49">
+        <v>1</v>
+      </c>
+      <c r="AW49">
+        <v>1</v>
+      </c>
     </row>
-    <row r="50" spans="1:46">
+    <row r="50" spans="1:49">
       <c r="A50" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C50">
         <v>34.0522</v>
@@ -7724,13 +8177,22 @@
       <c r="AT50">
         <v>1</v>
       </c>
+      <c r="AU50">
+        <v>1</v>
+      </c>
+      <c r="AV50">
+        <v>1</v>
+      </c>
+      <c r="AW50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="1:46">
+    <row r="51" spans="1:49">
       <c r="A51" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B51" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C51">
         <v>-33.8688</v>
@@ -7864,13 +8326,22 @@
       <c r="AT51">
         <v>4</v>
       </c>
+      <c r="AU51">
+        <v>4</v>
+      </c>
+      <c r="AV51">
+        <v>4</v>
+      </c>
+      <c r="AW51">
+        <v>4</v>
+      </c>
     </row>
-    <row r="52" spans="1:46">
+    <row r="52" spans="1:49">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B52" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C52">
         <v>-37.8136</v>
@@ -8004,13 +8475,22 @@
       <c r="AT52">
         <v>4</v>
       </c>
+      <c r="AU52">
+        <v>4</v>
+      </c>
+      <c r="AV52">
+        <v>4</v>
+      </c>
+      <c r="AW52">
+        <v>4</v>
+      </c>
     </row>
-    <row r="53" spans="1:46">
+    <row r="53" spans="1:49">
       <c r="A53" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B53" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C53">
         <v>-27.4698</v>
@@ -8144,10 +8624,19 @@
       <c r="AT53">
         <v>5</v>
       </c>
+      <c r="AU53">
+        <v>5</v>
+      </c>
+      <c r="AV53">
+        <v>5</v>
+      </c>
+      <c r="AW53">
+        <v>5</v>
+      </c>
     </row>
-    <row r="54" spans="1:46">
+    <row r="54" spans="1:49">
       <c r="B54" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C54">
         <v>12.5657</v>
@@ -8281,10 +8770,19 @@
       <c r="AT54">
         <v>1</v>
       </c>
+      <c r="AU54">
+        <v>1</v>
+      </c>
+      <c r="AV54">
+        <v>1</v>
+      </c>
+      <c r="AW54">
+        <v>1</v>
+      </c>
     </row>
-    <row r="55" spans="1:46">
+    <row r="55" spans="1:49">
       <c r="B55" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C55">
         <v>7.8731</v>
@@ -8418,10 +8916,19 @@
       <c r="AT55">
         <v>1</v>
       </c>
+      <c r="AU55">
+        <v>1</v>
+      </c>
+      <c r="AV55">
+        <v>1</v>
+      </c>
+      <c r="AW55">
+        <v>1</v>
+      </c>
     </row>
-    <row r="56" spans="1:46">
+    <row r="56" spans="1:49">
       <c r="B56" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C56">
         <v>51.1657</v>
@@ -8555,10 +9062,19 @@
       <c r="AT56">
         <v>16</v>
       </c>
+      <c r="AU56">
+        <v>16</v>
+      </c>
+      <c r="AV56">
+        <v>16</v>
+      </c>
+      <c r="AW56">
+        <v>16</v>
+      </c>
     </row>
-    <row r="57" spans="1:46">
+    <row r="57" spans="1:49">
       <c r="B57" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C57">
         <v>61.9241</v>
@@ -8692,10 +9208,19 @@
       <c r="AT57">
         <v>1</v>
       </c>
+      <c r="AU57">
+        <v>1</v>
+      </c>
+      <c r="AV57">
+        <v>1</v>
+      </c>
+      <c r="AW57">
+        <v>1</v>
+      </c>
     </row>
-    <row r="58" spans="1:46">
+    <row r="58" spans="1:49">
       <c r="B58" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C58">
         <v>23.4241</v>
@@ -8829,10 +9354,19 @@
       <c r="AT58">
         <v>8</v>
       </c>
+      <c r="AU58">
+        <v>8</v>
+      </c>
+      <c r="AV58">
+        <v>8</v>
+      </c>
+      <c r="AW58">
+        <v>8</v>
+      </c>
     </row>
-    <row r="59" spans="1:46">
+    <row r="59" spans="1:49">
       <c r="B59" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C59">
         <v>12.8797</v>
@@ -8966,10 +9500,19 @@
       <c r="AT59">
         <v>3</v>
       </c>
+      <c r="AU59">
+        <v>3</v>
+      </c>
+      <c r="AV59">
+        <v>3</v>
+      </c>
+      <c r="AW59">
+        <v>3</v>
+      </c>
     </row>
-    <row r="60" spans="1:46">
+    <row r="60" spans="1:49">
       <c r="B60" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C60">
         <v>20.5937</v>
@@ -9103,13 +9646,22 @@
       <c r="AT60">
         <v>3</v>
       </c>
+      <c r="AU60">
+        <v>3</v>
+      </c>
+      <c r="AV60">
+        <v>3</v>
+      </c>
+      <c r="AW60">
+        <v>3</v>
+      </c>
     </row>
-    <row r="61" spans="1:46">
+    <row r="61" spans="1:49">
       <c r="A61" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B61" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C61">
         <v>42.9849</v>
@@ -9243,10 +9795,19 @@
       <c r="AT61">
         <v>1</v>
       </c>
+      <c r="AU61">
+        <v>1</v>
+      </c>
+      <c r="AV61">
+        <v>1</v>
+      </c>
+      <c r="AW61">
+        <v>1</v>
+      </c>
     </row>
-    <row r="62" spans="1:46">
+    <row r="62" spans="1:49">
       <c r="B62" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C62">
         <v>41.8719</v>
@@ -9380,10 +9941,19 @@
       <c r="AT62">
         <v>3</v>
       </c>
+      <c r="AU62">
+        <v>3</v>
+      </c>
+      <c r="AV62">
+        <v>3</v>
+      </c>
+      <c r="AW62">
+        <v>3</v>
+      </c>
     </row>
-    <row r="63" spans="1:46">
+    <row r="63" spans="1:49">
       <c r="B63" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C63">
         <v>55.3781</v>
@@ -9517,10 +10087,19 @@
       <c r="AT63">
         <v>9</v>
       </c>
+      <c r="AU63">
+        <v>9</v>
+      </c>
+      <c r="AV63">
+        <v>9</v>
+      </c>
+      <c r="AW63">
+        <v>9</v>
+      </c>
     </row>
-    <row r="64" spans="1:46">
+    <row r="64" spans="1:49">
       <c r="B64" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C64">
         <v>61.524</v>
@@ -9654,10 +10233,19 @@
       <c r="AT64">
         <v>2</v>
       </c>
+      <c r="AU64">
+        <v>2</v>
+      </c>
+      <c r="AV64">
+        <v>2</v>
+      </c>
+      <c r="AW64">
+        <v>2</v>
+      </c>
     </row>
-    <row r="65" spans="1:46">
+    <row r="65" spans="1:49">
       <c r="B65" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C65">
         <v>60.1282</v>
@@ -9791,13 +10379,22 @@
       <c r="AT65">
         <v>1</v>
       </c>
+      <c r="AU65">
+        <v>1</v>
+      </c>
+      <c r="AV65">
+        <v>1</v>
+      </c>
+      <c r="AW65">
+        <v>1</v>
+      </c>
     </row>
-    <row r="66" spans="1:46">
+    <row r="66" spans="1:49">
       <c r="A66" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B66" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C66">
         <v>37.3541</v>
@@ -9931,10 +10528,19 @@
       <c r="AT66">
         <v>2</v>
       </c>
+      <c r="AU66">
+        <v>2</v>
+      </c>
+      <c r="AV66">
+        <v>2</v>
+      </c>
+      <c r="AW66">
+        <v>2</v>
+      </c>
     </row>
-    <row r="67" spans="1:46">
+    <row r="67" spans="1:49">
       <c r="B67" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C67">
         <v>40.4637</v>
@@ -10068,13 +10674,22 @@
       <c r="AT67">
         <v>2</v>
       </c>
+      <c r="AU67">
+        <v>2</v>
+      </c>
+      <c r="AV67">
+        <v>2</v>
+      </c>
+      <c r="AW67">
+        <v>2</v>
+      </c>
     </row>
-    <row r="68" spans="1:46">
+    <row r="68" spans="1:49">
       <c r="A68" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B68" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C68">
         <v>-34.9285</v>
@@ -10208,13 +10823,22 @@
       <c r="AT68">
         <v>2</v>
       </c>
+      <c r="AU68">
+        <v>2</v>
+      </c>
+      <c r="AV68">
+        <v>2</v>
+      </c>
+      <c r="AW68">
+        <v>2</v>
+      </c>
     </row>
-    <row r="69" spans="1:46">
+    <row r="69" spans="1:49">
       <c r="A69" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B69" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C69">
         <v>42.3601</v>
@@ -10348,13 +10972,22 @@
       <c r="AT69">
         <v>1</v>
       </c>
+      <c r="AU69">
+        <v>1</v>
+      </c>
+      <c r="AV69">
+        <v>1</v>
+      </c>
+      <c r="AW69">
+        <v>1</v>
+      </c>
     </row>
-    <row r="70" spans="1:46">
+    <row r="70" spans="1:49">
       <c r="A70" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B70" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C70">
         <v>36.5761</v>
@@ -10488,10 +11121,19 @@
       <c r="AT70">
         <v>2</v>
       </c>
+      <c r="AU70">
+        <v>2</v>
+      </c>
+      <c r="AV70">
+        <v>2</v>
+      </c>
+      <c r="AW70">
+        <v>2</v>
+      </c>
     </row>
-    <row r="71" spans="1:46">
+    <row r="71" spans="1:49">
       <c r="B71" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C71">
         <v>50.5039</v>
@@ -10625,13 +11267,22 @@
       <c r="AT71">
         <v>1</v>
       </c>
+      <c r="AU71">
+        <v>1</v>
+      </c>
+      <c r="AV71">
+        <v>1</v>
+      </c>
+      <c r="AW71">
+        <v>1</v>
+      </c>
     </row>
-    <row r="72" spans="1:46">
+    <row r="72" spans="1:49">
       <c r="A72" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B72" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C72">
         <v>43.0731</v>
@@ -10765,13 +11416,22 @@
       <c r="AT72">
         <v>1</v>
       </c>
+      <c r="AU72">
+        <v>1</v>
+      </c>
+      <c r="AV72">
+        <v>1</v>
+      </c>
+      <c r="AW72">
+        <v>1</v>
+      </c>
     </row>
-    <row r="73" spans="1:46">
+    <row r="73" spans="1:49">
       <c r="A73" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B73" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C73">
         <v>35.4437</v>
@@ -10905,13 +11565,22 @@
       <c r="AT73">
         <v>175</v>
       </c>
+      <c r="AU73">
+        <v>175</v>
+      </c>
+      <c r="AV73">
+        <v>218</v>
+      </c>
+      <c r="AW73">
+        <v>218</v>
+      </c>
     </row>
-    <row r="74" spans="1:46">
+    <row r="74" spans="1:49">
       <c r="A74" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B74" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C74">
         <v>32.7157</v>
@@ -11043,6 +11712,164 @@
         <v>1</v>
       </c>
       <c r="AT74">
+        <v>1</v>
+      </c>
+      <c r="AU74">
+        <v>2</v>
+      </c>
+      <c r="AV74">
+        <v>2</v>
+      </c>
+      <c r="AW74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:49">
+      <c r="A75" t="s">
+        <v>101</v>
+      </c>
+      <c r="B75" t="s">
+        <v>106</v>
+      </c>
+      <c r="C75">
+        <v>29.4241</v>
+      </c>
+      <c r="D75">
+        <v>-98.4936</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <v>0</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+      <c r="N75">
+        <v>0</v>
+      </c>
+      <c r="O75">
+        <v>0</v>
+      </c>
+      <c r="P75">
+        <v>0</v>
+      </c>
+      <c r="Q75">
+        <v>0</v>
+      </c>
+      <c r="R75">
+        <v>0</v>
+      </c>
+      <c r="S75">
+        <v>0</v>
+      </c>
+      <c r="T75">
+        <v>0</v>
+      </c>
+      <c r="U75">
+        <v>0</v>
+      </c>
+      <c r="V75">
+        <v>0</v>
+      </c>
+      <c r="W75">
+        <v>0</v>
+      </c>
+      <c r="X75">
+        <v>0</v>
+      </c>
+      <c r="Y75">
+        <v>0</v>
+      </c>
+      <c r="Z75">
+        <v>0</v>
+      </c>
+      <c r="AA75">
+        <v>0</v>
+      </c>
+      <c r="AB75">
+        <v>0</v>
+      </c>
+      <c r="AC75">
+        <v>0</v>
+      </c>
+      <c r="AD75">
+        <v>0</v>
+      </c>
+      <c r="AE75">
+        <v>0</v>
+      </c>
+      <c r="AF75">
+        <v>0</v>
+      </c>
+      <c r="AG75">
+        <v>0</v>
+      </c>
+      <c r="AH75">
+        <v>0</v>
+      </c>
+      <c r="AI75">
+        <v>0</v>
+      </c>
+      <c r="AJ75">
+        <v>0</v>
+      </c>
+      <c r="AK75">
+        <v>0</v>
+      </c>
+      <c r="AL75">
+        <v>0</v>
+      </c>
+      <c r="AM75">
+        <v>0</v>
+      </c>
+      <c r="AN75">
+        <v>0</v>
+      </c>
+      <c r="AO75">
+        <v>0</v>
+      </c>
+      <c r="AP75">
+        <v>0</v>
+      </c>
+      <c r="AQ75">
+        <v>0</v>
+      </c>
+      <c r="AR75">
+        <v>0</v>
+      </c>
+      <c r="AS75">
+        <v>0</v>
+      </c>
+      <c r="AT75">
+        <v>0</v>
+      </c>
+      <c r="AU75">
+        <v>0</v>
+      </c>
+      <c r="AV75">
+        <v>1</v>
+      </c>
+      <c r="AW75">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix plots, create df where columns are countries, rows are dates
</commit_message>
<xml_diff>
--- a/COVID19-Confirmed.xlsx
+++ b/COVID19-Confirmed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="109">
   <si>
     <t>Province/State</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>2/14/20</t>
+  </si>
+  <si>
+    <t>2/15/20</t>
   </si>
   <si>
     <t>Anhui</t>
@@ -695,13 +698,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB76"/>
+  <dimension ref="A1:AC76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,13 +789,16 @@
       <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:28">
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C2">
         <v>31.82571</v>
@@ -872,13 +878,16 @@
       <c r="AB2">
         <v>934</v>
       </c>
-    </row>
-    <row r="3" spans="1:28">
+      <c r="AC2">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C3">
         <v>40.18238</v>
@@ -958,13 +967,16 @@
       <c r="AB3">
         <v>372</v>
       </c>
-    </row>
-    <row r="4" spans="1:28">
+      <c r="AC3">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C4">
         <v>30.05718</v>
@@ -1044,13 +1056,16 @@
       <c r="AB4">
         <v>537</v>
       </c>
-    </row>
-    <row r="5" spans="1:28">
+      <c r="AC4">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C5">
         <v>26.07783</v>
@@ -1130,13 +1145,16 @@
       <c r="AB5">
         <v>281</v>
       </c>
-    </row>
-    <row r="6" spans="1:28">
+      <c r="AC5">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C6">
         <v>36.0611</v>
@@ -1216,13 +1234,16 @@
       <c r="AB6">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:28">
+      <c r="AC6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C7">
         <v>23.33841</v>
@@ -1302,13 +1323,16 @@
       <c r="AB7">
         <v>1261</v>
       </c>
-    </row>
-    <row r="8" spans="1:28">
+      <c r="AC7">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C8">
         <v>23.82908</v>
@@ -1388,13 +1412,16 @@
       <c r="AB8">
         <v>226</v>
       </c>
-    </row>
-    <row r="9" spans="1:28">
+      <c r="AC8">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C9">
         <v>26.81536</v>
@@ -1474,13 +1501,16 @@
       <c r="AB9">
         <v>140</v>
       </c>
-    </row>
-    <row r="10" spans="1:28">
+      <c r="AC9">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C10">
         <v>19.19673</v>
@@ -1560,13 +1590,16 @@
       <c r="AB10">
         <v>159</v>
       </c>
-    </row>
-    <row r="11" spans="1:28">
+      <c r="AC10">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C11">
         <v>38.0428</v>
@@ -1646,13 +1679,16 @@
       <c r="AB11">
         <v>283</v>
       </c>
-    </row>
-    <row r="12" spans="1:28">
+      <c r="AC11">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C12">
         <v>47.86199999999999</v>
@@ -1732,13 +1768,16 @@
       <c r="AB12">
         <v>419</v>
       </c>
-    </row>
-    <row r="13" spans="1:28">
+      <c r="AC12">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C13">
         <v>33.88202</v>
@@ -1818,13 +1857,16 @@
       <c r="AB13">
         <v>1184</v>
       </c>
-    </row>
-    <row r="14" spans="1:28">
+      <c r="AC13">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C14">
         <v>30.97564</v>
@@ -1904,13 +1946,16 @@
       <c r="AB14">
         <v>54406</v>
       </c>
-    </row>
-    <row r="15" spans="1:28">
+      <c r="AC14">
+        <v>56249</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C15">
         <v>27.61041</v>
@@ -1990,13 +2035,16 @@
       <c r="AB15">
         <v>988</v>
       </c>
-    </row>
-    <row r="16" spans="1:28">
+      <c r="AC15">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C16">
         <v>44.09448</v>
@@ -2076,13 +2124,16 @@
       <c r="AB16">
         <v>65</v>
       </c>
-    </row>
-    <row r="17" spans="1:28">
+      <c r="AC16">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C17">
         <v>32.97027</v>
@@ -2162,13 +2213,16 @@
       <c r="AB17">
         <v>593</v>
       </c>
-    </row>
-    <row r="18" spans="1:28">
+      <c r="AC17">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C18">
         <v>27.61401</v>
@@ -2248,13 +2302,16 @@
       <c r="AB18">
         <v>900</v>
       </c>
-    </row>
-    <row r="19" spans="1:28">
+      <c r="AC18">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C19">
         <v>43.66657</v>
@@ -2334,13 +2391,16 @@
       <c r="AB19">
         <v>86</v>
       </c>
-    </row>
-    <row r="20" spans="1:28">
+      <c r="AC19">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C20">
         <v>41.29284000000001</v>
@@ -2420,13 +2480,16 @@
       <c r="AB20">
         <v>119</v>
       </c>
-    </row>
-    <row r="21" spans="1:28">
+      <c r="AC20">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C21">
         <v>37.26923</v>
@@ -2506,13 +2569,16 @@
       <c r="AB21">
         <v>67</v>
       </c>
-    </row>
-    <row r="22" spans="1:28">
+      <c r="AC21">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C22">
         <v>35.65945</v>
@@ -2592,13 +2658,16 @@
       <c r="AB22">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:28">
+      <c r="AC22">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C23">
         <v>35.19165</v>
@@ -2678,13 +2747,16 @@
       <c r="AB23">
         <v>230</v>
       </c>
-    </row>
-    <row r="24" spans="1:28">
+      <c r="AC23">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C24">
         <v>36.34377</v>
@@ -2764,13 +2836,16 @@
       <c r="AB24">
         <v>523</v>
       </c>
-    </row>
-    <row r="25" spans="1:28">
+      <c r="AC24">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C25">
         <v>31.20327</v>
@@ -2850,13 +2925,16 @@
       <c r="AB25">
         <v>318</v>
       </c>
-    </row>
-    <row r="26" spans="1:28">
+      <c r="AC25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C26">
         <v>37.57769</v>
@@ -2936,13 +3014,16 @@
       <c r="AB26">
         <v>127</v>
       </c>
-    </row>
-    <row r="27" spans="1:28">
+      <c r="AC26">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C27">
         <v>30.61714</v>
@@ -3022,13 +3103,16 @@
       <c r="AB27">
         <v>463</v>
       </c>
-    </row>
-    <row r="28" spans="1:28">
+      <c r="AC27">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C28">
         <v>39.29362</v>
@@ -3108,13 +3192,16 @@
       <c r="AB28">
         <v>120</v>
       </c>
-    </row>
-    <row r="29" spans="1:28">
+      <c r="AC28">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C29">
         <v>30.1534</v>
@@ -3194,13 +3281,16 @@
       <c r="AB29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:28">
+      <c r="AC29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C30">
         <v>41.11981</v>
@@ -3280,13 +3370,16 @@
       <c r="AB30">
         <v>65</v>
       </c>
-    </row>
-    <row r="31" spans="1:28">
+      <c r="AC30">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C31">
         <v>24.97411</v>
@@ -3366,13 +3459,16 @@
       <c r="AB31">
         <v>162</v>
       </c>
-    </row>
-    <row r="32" spans="1:28">
+      <c r="AC31">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C32">
         <v>29.18251</v>
@@ -3452,10 +3548,13 @@
       <c r="AB32">
         <v>1155</v>
       </c>
-    </row>
-    <row r="33" spans="1:28">
+      <c r="AC32">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29">
       <c r="B33" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C33">
         <v>13.7563</v>
@@ -3535,10 +3634,13 @@
       <c r="AB33">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:28">
+      <c r="AC33">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29">
       <c r="B34" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C34">
         <v>35.6762</v>
@@ -3618,10 +3720,13 @@
       <c r="AB34">
         <v>29</v>
       </c>
-    </row>
-    <row r="35" spans="1:28">
+      <c r="AC34">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29">
       <c r="B35" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C35">
         <v>37.5665</v>
@@ -3701,13 +3806,16 @@
       <c r="AB35">
         <v>28</v>
       </c>
-    </row>
-    <row r="36" spans="1:28">
+      <c r="AC35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C36">
         <v>23.6978</v>
@@ -3787,13 +3895,16 @@
       <c r="AB36">
         <v>18</v>
       </c>
-    </row>
-    <row r="37" spans="1:28">
+      <c r="AC36">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C37">
         <v>47.7511</v>
@@ -3802,34 +3913,34 @@
         <v>-120.74</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O37">
         <v>1</v>
@@ -3873,13 +3984,16 @@
       <c r="AB37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:28">
+      <c r="AC37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C38">
         <v>40.6331</v>
@@ -3894,28 +4008,28 @@
         <v>0</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O38">
         <v>2</v>
@@ -3959,13 +4073,16 @@
       <c r="AB38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:28">
+      <c r="AC38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C39">
         <v>34.0489</v>
@@ -3986,22 +4103,22 @@
         <v>0</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O39">
         <v>1</v>
@@ -4045,13 +4162,16 @@
       <c r="AB39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:28">
+      <c r="AC39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C40">
         <v>22.1987</v>
@@ -4131,13 +4251,16 @@
       <c r="AB40">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:28">
+      <c r="AC40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B41" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C41">
         <v>22.3193</v>
@@ -4217,10 +4340,13 @@
       <c r="AB41">
         <v>56</v>
       </c>
-    </row>
-    <row r="42" spans="1:28">
+      <c r="AC41">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29">
       <c r="B42" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C42">
         <v>1.3521</v>
@@ -4232,28 +4358,28 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I42">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J42">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K42">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L42">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M42">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N42">
         <v>13</v>
@@ -4300,10 +4426,13 @@
       <c r="AB42">
         <v>67</v>
       </c>
-    </row>
-    <row r="43" spans="1:28">
+      <c r="AC42">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29">
       <c r="B43" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C43">
         <v>21.0278</v>
@@ -4383,10 +4512,13 @@
       <c r="AB43">
         <v>16</v>
       </c>
-    </row>
-    <row r="44" spans="1:28">
+      <c r="AC43">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29">
       <c r="B44" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C44">
         <v>46.2276</v>
@@ -4466,10 +4598,13 @@
       <c r="AB44">
         <v>11</v>
       </c>
-    </row>
-    <row r="45" spans="1:28">
+      <c r="AC44">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29">
       <c r="B45" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C45">
         <v>28.3949</v>
@@ -4549,10 +4684,13 @@
       <c r="AB45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:28">
+      <c r="AC45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29">
       <c r="B46" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C46">
         <v>4.2105</v>
@@ -4570,22 +4708,22 @@
         <v>0</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J46">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K46">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L46">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M46">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N46">
         <v>8</v>
@@ -4632,13 +4770,16 @@
       <c r="AB46">
         <v>19</v>
       </c>
-    </row>
-    <row r="47" spans="1:28">
+      <c r="AC46">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C47">
         <v>43.6532</v>
@@ -4659,31 +4800,31 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R47">
         <v>2</v>
@@ -4718,13 +4859,16 @@
       <c r="AB47">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:28">
+      <c r="AC47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29">
       <c r="A48" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B48" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C48">
         <v>49.2827</v>
@@ -4804,13 +4948,16 @@
       <c r="AB48">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:28">
+      <c r="AC48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B49" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C49">
         <v>33.7879</v>
@@ -4831,22 +4978,22 @@
         <v>0</v>
       </c>
       <c r="I49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O49">
         <v>1</v>
@@ -4890,13 +5037,16 @@
       <c r="AB49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:28">
+      <c r="AC49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29">
       <c r="A50" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B50" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C50">
         <v>34.0522</v>
@@ -4917,22 +5067,22 @@
         <v>0</v>
       </c>
       <c r="I50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O50">
         <v>1</v>
@@ -4976,13 +5126,16 @@
       <c r="AB50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:28">
+      <c r="AC50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29">
       <c r="A51" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B51" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C51">
         <v>-33.8688</v>
@@ -5003,7 +5156,7 @@
         <v>0</v>
       </c>
       <c r="I51">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J51">
         <v>4</v>
@@ -5062,13 +5215,16 @@
       <c r="AB51">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:28">
+      <c r="AC51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29">
       <c r="A52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B52" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C52">
         <v>-37.8136</v>
@@ -5089,7 +5245,7 @@
         <v>0</v>
       </c>
       <c r="I52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52">
         <v>1</v>
@@ -5148,13 +5304,16 @@
       <c r="AB52">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:28">
+      <c r="AC52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29">
       <c r="A53" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B53" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C53">
         <v>-27.4698</v>
@@ -5184,7 +5343,7 @@
         <v>0</v>
       </c>
       <c r="L53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M53">
         <v>3</v>
@@ -5234,10 +5393,13 @@
       <c r="AB53">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:28">
+      <c r="AC53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:29">
       <c r="B54" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C54">
         <v>12.5657</v>
@@ -5317,10 +5479,13 @@
       <c r="AB54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:28">
+      <c r="AC54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:29">
       <c r="B55" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C55">
         <v>7.8731</v>
@@ -5400,10 +5565,13 @@
       <c r="AB55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:28">
+      <c r="AC55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29">
       <c r="B56" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C56">
         <v>51.1657</v>
@@ -5427,19 +5595,19 @@
         <v>0</v>
       </c>
       <c r="J56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K56">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L56">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M56">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N56">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O56">
         <v>8</v>
@@ -5483,10 +5651,13 @@
       <c r="AB56">
         <v>16</v>
       </c>
-    </row>
-    <row r="57" spans="1:28">
+      <c r="AC56">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29">
       <c r="B57" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C57">
         <v>61.9241</v>
@@ -5566,10 +5737,13 @@
       <c r="AB57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:28">
+      <c r="AC57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29">
       <c r="B58" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C58">
         <v>23.4241</v>
@@ -5649,10 +5823,13 @@
       <c r="AB58">
         <v>8</v>
       </c>
-    </row>
-    <row r="59" spans="1:28">
+      <c r="AC58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29">
       <c r="B59" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C59">
         <v>12.8797</v>
@@ -5732,10 +5909,13 @@
       <c r="AB59">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="1:28">
+      <c r="AC59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29">
       <c r="B60" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C60">
         <v>20.5937</v>
@@ -5815,13 +5995,16 @@
       <c r="AB60">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:28">
+      <c r="AC60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29">
       <c r="A61" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B61" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C61">
         <v>42.9849</v>
@@ -5857,16 +6040,16 @@
         <v>0</v>
       </c>
       <c r="N61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R61">
         <v>1</v>
@@ -5901,10 +6084,13 @@
       <c r="AB61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:28">
+      <c r="AC61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29">
       <c r="B62" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C62">
         <v>41.8719</v>
@@ -5984,10 +6170,13 @@
       <c r="AB62">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:28">
+      <c r="AC62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:29">
       <c r="B63" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C63">
         <v>55.3781</v>
@@ -6067,10 +6256,13 @@
       <c r="AB63">
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="1:28">
+      <c r="AC63">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:29">
       <c r="B64" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C64">
         <v>61.52399999999999</v>
@@ -6150,10 +6342,13 @@
       <c r="AB64">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="1:28">
+      <c r="AC64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:29">
       <c r="B65" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C65">
         <v>60.1282</v>
@@ -6233,13 +6428,16 @@
       <c r="AB65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:28">
+      <c r="AC65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:29">
       <c r="A66" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B66" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C66">
         <v>37.3541</v>
@@ -6275,7 +6473,7 @@
         <v>0</v>
       </c>
       <c r="N66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O66">
         <v>1</v>
@@ -6319,10 +6517,13 @@
       <c r="AB66">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:28">
+      <c r="AC66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:29">
       <c r="B67" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C67">
         <v>40.4637</v>
@@ -6402,13 +6603,16 @@
       <c r="AB67">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:28">
+      <c r="AC67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:29">
       <c r="A68" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B68" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C68">
         <v>-34.9285</v>
@@ -6488,13 +6692,16 @@
       <c r="AB68">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:28">
+      <c r="AC68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:29">
       <c r="A69" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B69" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C69">
         <v>42.3601</v>
@@ -6574,13 +6781,16 @@
       <c r="AB69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:28">
+      <c r="AC69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:29">
       <c r="A70" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B70" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C70">
         <v>36.5761</v>
@@ -6660,10 +6870,13 @@
       <c r="AB70">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:28">
+      <c r="AC70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:29">
       <c r="B71" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C71">
         <v>50.5039</v>
@@ -6743,13 +6956,16 @@
       <c r="AB71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:28">
+      <c r="AC71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:29">
       <c r="A72" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C72">
         <v>43.0731</v>
@@ -6829,13 +7045,16 @@
       <c r="AB72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:28">
+      <c r="AC72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B73" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C73">
         <v>35.4437</v>
@@ -6892,10 +7111,10 @@
         <v>0</v>
       </c>
       <c r="U73">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="V73">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="W73">
         <v>64</v>
@@ -6915,13 +7134,16 @@
       <c r="AB73">
         <v>218</v>
       </c>
-    </row>
-    <row r="74" spans="1:28">
+      <c r="AC73">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B74" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C74">
         <v>32.7157</v>
@@ -7001,13 +7223,16 @@
       <c r="AB74">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:28">
+      <c r="AC74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:29">
       <c r="A75" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C75">
         <v>29.4241</v>
@@ -7087,10 +7312,13 @@
       <c r="AB75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:28">
+      <c r="AC75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:29">
       <c r="B76" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C76">
         <v>26.8206</v>
@@ -7168,6 +7396,9 @@
         <v>0</v>
       </c>
       <c r="AB76">
+        <v>1</v>
+      </c>
+      <c r="AC76">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update charts and tables, check if everything works
</commit_message>
<xml_diff>
--- a/COVID19-Confirmed.xlsx
+++ b/COVID19-Confirmed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="111">
   <si>
     <t>Province/State</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>2/15/20</t>
+  </si>
+  <si>
+    <t>2/16/20</t>
+  </si>
+  <si>
+    <t>2/17/20</t>
   </si>
   <si>
     <t>Anhui</t>
@@ -698,13 +704,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC76"/>
+  <dimension ref="A1:AE76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:31">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -792,13 +798,19 @@
       <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:31">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C2">
         <v>31.82571</v>
@@ -881,13 +893,19 @@
       <c r="AC2">
         <v>950</v>
       </c>
+      <c r="AD2">
+        <v>962</v>
+      </c>
+      <c r="AE2">
+        <v>973</v>
+      </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:31">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C3">
         <v>40.18238</v>
@@ -970,13 +988,19 @@
       <c r="AC3">
         <v>375</v>
       </c>
+      <c r="AD3">
+        <v>380</v>
+      </c>
+      <c r="AE3">
+        <v>381</v>
+      </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:31">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C4">
         <v>30.05718</v>
@@ -1059,13 +1083,19 @@
       <c r="AC4">
         <v>544</v>
       </c>
+      <c r="AD4">
+        <v>551</v>
+      </c>
+      <c r="AE4">
+        <v>553</v>
+      </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:31">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C5">
         <v>26.07783</v>
@@ -1148,13 +1178,19 @@
       <c r="AC5">
         <v>285</v>
       </c>
+      <c r="AD5">
+        <v>287</v>
+      </c>
+      <c r="AE5">
+        <v>290</v>
+      </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:31">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C6">
         <v>36.0611</v>
@@ -1237,13 +1273,19 @@
       <c r="AC6">
         <v>90</v>
       </c>
+      <c r="AD6">
+        <v>90</v>
+      </c>
+      <c r="AE6">
+        <v>91</v>
+      </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:31">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C7">
         <v>23.33841</v>
@@ -1326,13 +1368,19 @@
       <c r="AC7">
         <v>1294</v>
       </c>
+      <c r="AD7">
+        <v>1316</v>
+      </c>
+      <c r="AE7">
+        <v>1322</v>
+      </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:31">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C8">
         <v>23.82908</v>
@@ -1415,13 +1463,19 @@
       <c r="AC8">
         <v>235</v>
       </c>
+      <c r="AD8">
+        <v>237</v>
+      </c>
+      <c r="AE8">
+        <v>238</v>
+      </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:31">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C9">
         <v>26.81536</v>
@@ -1504,13 +1558,19 @@
       <c r="AC9">
         <v>143</v>
       </c>
+      <c r="AD9">
+        <v>144</v>
+      </c>
+      <c r="AE9">
+        <v>146</v>
+      </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:31">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C10">
         <v>19.19673</v>
@@ -1593,13 +1653,19 @@
       <c r="AC10">
         <v>162</v>
       </c>
+      <c r="AD10">
+        <v>162</v>
+      </c>
+      <c r="AE10">
+        <v>163</v>
+      </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:31">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C11">
         <v>38.0428</v>
@@ -1682,13 +1748,19 @@
       <c r="AC11">
         <v>291</v>
       </c>
+      <c r="AD11">
+        <v>300</v>
+      </c>
+      <c r="AE11">
+        <v>301</v>
+      </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:31">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C12">
         <v>47.86199999999999</v>
@@ -1771,13 +1843,19 @@
       <c r="AC12">
         <v>425</v>
       </c>
+      <c r="AD12">
+        <v>445</v>
+      </c>
+      <c r="AE12">
+        <v>457</v>
+      </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:31">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C13">
         <v>33.88202</v>
@@ -1860,13 +1938,19 @@
       <c r="AC13">
         <v>1212</v>
       </c>
+      <c r="AD13">
+        <v>1231</v>
+      </c>
+      <c r="AE13">
+        <v>1246</v>
+      </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:31">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C14">
         <v>30.97564</v>
@@ -1949,13 +2033,19 @@
       <c r="AC14">
         <v>56249</v>
       </c>
+      <c r="AD14">
+        <v>58182</v>
+      </c>
+      <c r="AE14">
+        <v>59989</v>
+      </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:31">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C15">
         <v>27.61041</v>
@@ -2038,13 +2128,19 @@
       <c r="AC15">
         <v>1001</v>
       </c>
+      <c r="AD15">
+        <v>1004</v>
+      </c>
+      <c r="AE15">
+        <v>1006</v>
+      </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:31">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C16">
         <v>44.09448</v>
@@ -2127,13 +2223,19 @@
       <c r="AC16">
         <v>68</v>
       </c>
+      <c r="AD16">
+        <v>70</v>
+      </c>
+      <c r="AE16">
+        <v>72</v>
+      </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:31">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C17">
         <v>32.97027</v>
@@ -2216,13 +2318,19 @@
       <c r="AC17">
         <v>604</v>
       </c>
+      <c r="AD17">
+        <v>617</v>
+      </c>
+      <c r="AE17">
+        <v>626</v>
+      </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:31">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C18">
         <v>27.61401</v>
@@ -2305,13 +2413,19 @@
       <c r="AC18">
         <v>913</v>
       </c>
+      <c r="AD18">
+        <v>925</v>
+      </c>
+      <c r="AE18">
+        <v>930</v>
+      </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:31">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C19">
         <v>43.66657</v>
@@ -2394,13 +2508,19 @@
       <c r="AC19">
         <v>88</v>
       </c>
+      <c r="AD19">
+        <v>89</v>
+      </c>
+      <c r="AE19">
+        <v>89</v>
+      </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:31">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C20">
         <v>41.29284000000001</v>
@@ -2483,13 +2603,19 @@
       <c r="AC20">
         <v>119</v>
       </c>
+      <c r="AD20">
+        <v>121</v>
+      </c>
+      <c r="AE20">
+        <v>121</v>
+      </c>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:31">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C21">
         <v>37.26923</v>
@@ -2572,13 +2698,19 @@
       <c r="AC21">
         <v>70</v>
       </c>
+      <c r="AD21">
+        <v>70</v>
+      </c>
+      <c r="AE21">
+        <v>70</v>
+      </c>
     </row>
-    <row r="22" spans="1:29">
+    <row r="22" spans="1:31">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C22">
         <v>35.65945</v>
@@ -2661,13 +2793,19 @@
       <c r="AC22">
         <v>18</v>
       </c>
+      <c r="AD22">
+        <v>18</v>
+      </c>
+      <c r="AE22">
+        <v>18</v>
+      </c>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:31">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C23">
         <v>35.19165</v>
@@ -2750,13 +2888,19 @@
       <c r="AC23">
         <v>232</v>
       </c>
+      <c r="AD23">
+        <v>236</v>
+      </c>
+      <c r="AE23">
+        <v>240</v>
+      </c>
     </row>
-    <row r="24" spans="1:29">
+    <row r="24" spans="1:31">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C24">
         <v>36.34377</v>
@@ -2839,13 +2983,19 @@
       <c r="AC24">
         <v>532</v>
       </c>
+      <c r="AD24">
+        <v>537</v>
+      </c>
+      <c r="AE24">
+        <v>541</v>
+      </c>
     </row>
-    <row r="25" spans="1:29">
+    <row r="25" spans="1:31">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C25">
         <v>31.20327</v>
@@ -2928,13 +3078,19 @@
       <c r="AC25">
         <v>326</v>
       </c>
+      <c r="AD25">
+        <v>328</v>
+      </c>
+      <c r="AE25">
+        <v>333</v>
+      </c>
     </row>
-    <row r="26" spans="1:29">
+    <row r="26" spans="1:31">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C26">
         <v>37.57769</v>
@@ -3017,13 +3173,19 @@
       <c r="AC26">
         <v>128</v>
       </c>
+      <c r="AD26">
+        <v>129</v>
+      </c>
+      <c r="AE26">
+        <v>130</v>
+      </c>
     </row>
-    <row r="27" spans="1:29">
+    <row r="27" spans="1:31">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C27">
         <v>30.61714</v>
@@ -3106,13 +3268,19 @@
       <c r="AC27">
         <v>470</v>
       </c>
+      <c r="AD27">
+        <v>481</v>
+      </c>
+      <c r="AE27">
+        <v>495</v>
+      </c>
     </row>
-    <row r="28" spans="1:29">
+    <row r="28" spans="1:31">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C28">
         <v>39.29362</v>
@@ -3195,13 +3363,19 @@
       <c r="AC28">
         <v>122</v>
       </c>
+      <c r="AD28">
+        <v>124</v>
+      </c>
+      <c r="AE28">
+        <v>125</v>
+      </c>
     </row>
-    <row r="29" spans="1:29">
+    <row r="29" spans="1:31">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C29">
         <v>30.1534</v>
@@ -3284,13 +3458,19 @@
       <c r="AC29">
         <v>1</v>
       </c>
+      <c r="AD29">
+        <v>1</v>
+      </c>
+      <c r="AE29">
+        <v>1</v>
+      </c>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:31">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C30">
         <v>41.11981</v>
@@ -3373,13 +3553,19 @@
       <c r="AC30">
         <v>70</v>
       </c>
+      <c r="AD30">
+        <v>71</v>
+      </c>
+      <c r="AE30">
+        <v>75</v>
+      </c>
     </row>
-    <row r="31" spans="1:29">
+    <row r="31" spans="1:31">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C31">
         <v>24.97411</v>
@@ -3462,13 +3648,19 @@
       <c r="AC31">
         <v>168</v>
       </c>
+      <c r="AD31">
+        <v>171</v>
+      </c>
+      <c r="AE31">
+        <v>171</v>
+      </c>
     </row>
-    <row r="32" spans="1:29">
+    <row r="32" spans="1:31">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C32">
         <v>29.18251</v>
@@ -3551,10 +3743,16 @@
       <c r="AC32">
         <v>1162</v>
       </c>
+      <c r="AD32">
+        <v>1167</v>
+      </c>
+      <c r="AE32">
+        <v>1171</v>
+      </c>
     </row>
-    <row r="33" spans="1:29">
+    <row r="33" spans="1:31">
       <c r="B33" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C33">
         <v>13.7563</v>
@@ -3637,10 +3835,16 @@
       <c r="AC33">
         <v>33</v>
       </c>
+      <c r="AD33">
+        <v>34</v>
+      </c>
+      <c r="AE33">
+        <v>35</v>
+      </c>
     </row>
-    <row r="34" spans="1:29">
+    <row r="34" spans="1:31">
       <c r="B34" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C34">
         <v>35.6762</v>
@@ -3723,10 +3927,16 @@
       <c r="AC34">
         <v>43</v>
       </c>
+      <c r="AD34">
+        <v>59</v>
+      </c>
+      <c r="AE34">
+        <v>66</v>
+      </c>
     </row>
-    <row r="35" spans="1:29">
+    <row r="35" spans="1:31">
       <c r="B35" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C35">
         <v>37.5665</v>
@@ -3809,13 +4019,19 @@
       <c r="AC35">
         <v>28</v>
       </c>
+      <c r="AD35">
+        <v>29</v>
+      </c>
+      <c r="AE35">
+        <v>30</v>
+      </c>
     </row>
-    <row r="36" spans="1:29">
+    <row r="36" spans="1:31">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C36">
         <v>23.6978</v>
@@ -3898,13 +4114,19 @@
       <c r="AC36">
         <v>18</v>
       </c>
+      <c r="AD36">
+        <v>20</v>
+      </c>
+      <c r="AE36">
+        <v>22</v>
+      </c>
     </row>
-    <row r="37" spans="1:29">
+    <row r="37" spans="1:31">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C37">
         <v>47.7511</v>
@@ -3987,13 +4209,19 @@
       <c r="AC37">
         <v>1</v>
       </c>
+      <c r="AD37">
+        <v>1</v>
+      </c>
+      <c r="AE37">
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="1:29">
+    <row r="38" spans="1:31">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C38">
         <v>40.6331</v>
@@ -4076,13 +4304,19 @@
       <c r="AC38">
         <v>2</v>
       </c>
+      <c r="AD38">
+        <v>2</v>
+      </c>
+      <c r="AE38">
+        <v>2</v>
+      </c>
     </row>
-    <row r="39" spans="1:29">
+    <row r="39" spans="1:31">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C39">
         <v>34.0489</v>
@@ -4165,13 +4399,19 @@
       <c r="AC39">
         <v>1</v>
       </c>
+      <c r="AD39">
+        <v>1</v>
+      </c>
+      <c r="AE39">
+        <v>1</v>
+      </c>
     </row>
-    <row r="40" spans="1:29">
+    <row r="40" spans="1:31">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B40" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C40">
         <v>22.1987</v>
@@ -4254,13 +4494,19 @@
       <c r="AC40">
         <v>10</v>
       </c>
+      <c r="AD40">
+        <v>10</v>
+      </c>
+      <c r="AE40">
+        <v>10</v>
+      </c>
     </row>
-    <row r="41" spans="1:29">
+    <row r="41" spans="1:31">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C41">
         <v>22.3193</v>
@@ -4343,10 +4589,16 @@
       <c r="AC41">
         <v>56</v>
       </c>
+      <c r="AD41">
+        <v>57</v>
+      </c>
+      <c r="AE41">
+        <v>60</v>
+      </c>
     </row>
-    <row r="42" spans="1:29">
+    <row r="42" spans="1:31">
       <c r="B42" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C42">
         <v>1.3521</v>
@@ -4429,10 +4681,16 @@
       <c r="AC42">
         <v>72</v>
       </c>
+      <c r="AD42">
+        <v>75</v>
+      </c>
+      <c r="AE42">
+        <v>77</v>
+      </c>
     </row>
-    <row r="43" spans="1:29">
+    <row r="43" spans="1:31">
       <c r="B43" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C43">
         <v>21.0278</v>
@@ -4515,10 +4773,16 @@
       <c r="AC43">
         <v>16</v>
       </c>
+      <c r="AD43">
+        <v>16</v>
+      </c>
+      <c r="AE43">
+        <v>16</v>
+      </c>
     </row>
-    <row r="44" spans="1:29">
+    <row r="44" spans="1:31">
       <c r="B44" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C44">
         <v>46.2276</v>
@@ -4601,10 +4865,16 @@
       <c r="AC44">
         <v>12</v>
       </c>
+      <c r="AD44">
+        <v>12</v>
+      </c>
+      <c r="AE44">
+        <v>12</v>
+      </c>
     </row>
-    <row r="45" spans="1:29">
+    <row r="45" spans="1:31">
       <c r="B45" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C45">
         <v>28.3949</v>
@@ -4687,10 +4957,16 @@
       <c r="AC45">
         <v>1</v>
       </c>
+      <c r="AD45">
+        <v>1</v>
+      </c>
+      <c r="AE45">
+        <v>1</v>
+      </c>
     </row>
-    <row r="46" spans="1:29">
+    <row r="46" spans="1:31">
       <c r="B46" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C46">
         <v>4.2105</v>
@@ -4773,13 +5049,19 @@
       <c r="AC46">
         <v>22</v>
       </c>
+      <c r="AD46">
+        <v>22</v>
+      </c>
+      <c r="AE46">
+        <v>22</v>
+      </c>
     </row>
-    <row r="47" spans="1:29">
+    <row r="47" spans="1:31">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C47">
         <v>43.6532</v>
@@ -4862,13 +5144,19 @@
       <c r="AC47">
         <v>2</v>
       </c>
+      <c r="AD47">
+        <v>2</v>
+      </c>
+      <c r="AE47">
+        <v>2</v>
+      </c>
     </row>
-    <row r="48" spans="1:29">
+    <row r="48" spans="1:31">
       <c r="A48" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C48">
         <v>49.2827</v>
@@ -4951,13 +5239,19 @@
       <c r="AC48">
         <v>4</v>
       </c>
+      <c r="AD48">
+        <v>4</v>
+      </c>
+      <c r="AE48">
+        <v>5</v>
+      </c>
     </row>
-    <row r="49" spans="1:29">
+    <row r="49" spans="1:31">
       <c r="A49" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C49">
         <v>33.7879</v>
@@ -5040,13 +5334,19 @@
       <c r="AC49">
         <v>1</v>
       </c>
+      <c r="AD49">
+        <v>1</v>
+      </c>
+      <c r="AE49">
+        <v>1</v>
+      </c>
     </row>
-    <row r="50" spans="1:29">
+    <row r="50" spans="1:31">
       <c r="A50" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B50" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C50">
         <v>34.0522</v>
@@ -5129,13 +5429,19 @@
       <c r="AC50">
         <v>1</v>
       </c>
+      <c r="AD50">
+        <v>1</v>
+      </c>
+      <c r="AE50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="1:29">
+    <row r="51" spans="1:31">
       <c r="A51" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B51" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C51">
         <v>-33.8688</v>
@@ -5218,13 +5524,19 @@
       <c r="AC51">
         <v>4</v>
       </c>
+      <c r="AD51">
+        <v>4</v>
+      </c>
+      <c r="AE51">
+        <v>4</v>
+      </c>
     </row>
-    <row r="52" spans="1:29">
+    <row r="52" spans="1:31">
       <c r="A52" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B52" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C52">
         <v>-37.8136</v>
@@ -5307,13 +5619,19 @@
       <c r="AC52">
         <v>4</v>
       </c>
+      <c r="AD52">
+        <v>4</v>
+      </c>
+      <c r="AE52">
+        <v>4</v>
+      </c>
     </row>
-    <row r="53" spans="1:29">
+    <row r="53" spans="1:31">
       <c r="A53" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C53">
         <v>-27.4698</v>
@@ -5396,10 +5714,16 @@
       <c r="AC53">
         <v>5</v>
       </c>
+      <c r="AD53">
+        <v>5</v>
+      </c>
+      <c r="AE53">
+        <v>5</v>
+      </c>
     </row>
-    <row r="54" spans="1:29">
+    <row r="54" spans="1:31">
       <c r="B54" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C54">
         <v>12.5657</v>
@@ -5482,10 +5806,16 @@
       <c r="AC54">
         <v>1</v>
       </c>
+      <c r="AD54">
+        <v>1</v>
+      </c>
+      <c r="AE54">
+        <v>1</v>
+      </c>
     </row>
-    <row r="55" spans="1:29">
+    <row r="55" spans="1:31">
       <c r="B55" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C55">
         <v>7.8731</v>
@@ -5568,10 +5898,16 @@
       <c r="AC55">
         <v>1</v>
       </c>
+      <c r="AD55">
+        <v>1</v>
+      </c>
+      <c r="AE55">
+        <v>1</v>
+      </c>
     </row>
-    <row r="56" spans="1:29">
+    <row r="56" spans="1:31">
       <c r="B56" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C56">
         <v>51.1657</v>
@@ -5654,10 +5990,16 @@
       <c r="AC56">
         <v>16</v>
       </c>
+      <c r="AD56">
+        <v>16</v>
+      </c>
+      <c r="AE56">
+        <v>16</v>
+      </c>
     </row>
-    <row r="57" spans="1:29">
+    <row r="57" spans="1:31">
       <c r="B57" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C57">
         <v>61.9241</v>
@@ -5740,10 +6082,16 @@
       <c r="AC57">
         <v>1</v>
       </c>
+      <c r="AD57">
+        <v>1</v>
+      </c>
+      <c r="AE57">
+        <v>1</v>
+      </c>
     </row>
-    <row r="58" spans="1:29">
+    <row r="58" spans="1:31">
       <c r="B58" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C58">
         <v>23.4241</v>
@@ -5826,10 +6174,16 @@
       <c r="AC58">
         <v>8</v>
       </c>
+      <c r="AD58">
+        <v>9</v>
+      </c>
+      <c r="AE58">
+        <v>9</v>
+      </c>
     </row>
-    <row r="59" spans="1:29">
+    <row r="59" spans="1:31">
       <c r="B59" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C59">
         <v>12.8797</v>
@@ -5912,10 +6266,16 @@
       <c r="AC59">
         <v>3</v>
       </c>
+      <c r="AD59">
+        <v>3</v>
+      </c>
+      <c r="AE59">
+        <v>3</v>
+      </c>
     </row>
-    <row r="60" spans="1:29">
+    <row r="60" spans="1:31">
       <c r="B60" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C60">
         <v>20.5937</v>
@@ -5998,13 +6358,19 @@
       <c r="AC60">
         <v>3</v>
       </c>
+      <c r="AD60">
+        <v>3</v>
+      </c>
+      <c r="AE60">
+        <v>3</v>
+      </c>
     </row>
-    <row r="61" spans="1:29">
+    <row r="61" spans="1:31">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B61" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C61">
         <v>42.9849</v>
@@ -6087,10 +6453,16 @@
       <c r="AC61">
         <v>1</v>
       </c>
+      <c r="AD61">
+        <v>1</v>
+      </c>
+      <c r="AE61">
+        <v>1</v>
+      </c>
     </row>
-    <row r="62" spans="1:29">
+    <row r="62" spans="1:31">
       <c r="B62" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C62">
         <v>41.8719</v>
@@ -6173,10 +6545,16 @@
       <c r="AC62">
         <v>3</v>
       </c>
+      <c r="AD62">
+        <v>3</v>
+      </c>
+      <c r="AE62">
+        <v>3</v>
+      </c>
     </row>
-    <row r="63" spans="1:29">
+    <row r="63" spans="1:31">
       <c r="B63" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C63">
         <v>55.3781</v>
@@ -6259,10 +6637,16 @@
       <c r="AC63">
         <v>9</v>
       </c>
+      <c r="AD63">
+        <v>9</v>
+      </c>
+      <c r="AE63">
+        <v>9</v>
+      </c>
     </row>
-    <row r="64" spans="1:29">
+    <row r="64" spans="1:31">
       <c r="B64" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C64">
         <v>61.52399999999999</v>
@@ -6345,10 +6729,16 @@
       <c r="AC64">
         <v>2</v>
       </c>
+      <c r="AD64">
+        <v>2</v>
+      </c>
+      <c r="AE64">
+        <v>2</v>
+      </c>
     </row>
-    <row r="65" spans="1:29">
+    <row r="65" spans="1:31">
       <c r="B65" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C65">
         <v>60.1282</v>
@@ -6431,13 +6821,19 @@
       <c r="AC65">
         <v>1</v>
       </c>
+      <c r="AD65">
+        <v>1</v>
+      </c>
+      <c r="AE65">
+        <v>1</v>
+      </c>
     </row>
-    <row r="66" spans="1:29">
+    <row r="66" spans="1:31">
       <c r="A66" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C66">
         <v>37.3541</v>
@@ -6520,10 +6916,16 @@
       <c r="AC66">
         <v>2</v>
       </c>
+      <c r="AD66">
+        <v>2</v>
+      </c>
+      <c r="AE66">
+        <v>2</v>
+      </c>
     </row>
-    <row r="67" spans="1:29">
+    <row r="67" spans="1:31">
       <c r="B67" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C67">
         <v>40.4637</v>
@@ -6606,13 +7008,19 @@
       <c r="AC67">
         <v>2</v>
       </c>
+      <c r="AD67">
+        <v>2</v>
+      </c>
+      <c r="AE67">
+        <v>2</v>
+      </c>
     </row>
-    <row r="68" spans="1:29">
+    <row r="68" spans="1:31">
       <c r="A68" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B68" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C68">
         <v>-34.9285</v>
@@ -6695,13 +7103,19 @@
       <c r="AC68">
         <v>2</v>
       </c>
+      <c r="AD68">
+        <v>2</v>
+      </c>
+      <c r="AE68">
+        <v>2</v>
+      </c>
     </row>
-    <row r="69" spans="1:29">
+    <row r="69" spans="1:31">
       <c r="A69" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B69" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C69">
         <v>42.3601</v>
@@ -6784,13 +7198,19 @@
       <c r="AC69">
         <v>1</v>
       </c>
+      <c r="AD69">
+        <v>1</v>
+      </c>
+      <c r="AE69">
+        <v>1</v>
+      </c>
     </row>
-    <row r="70" spans="1:29">
+    <row r="70" spans="1:31">
       <c r="A70" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B70" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C70">
         <v>36.5761</v>
@@ -6873,10 +7293,16 @@
       <c r="AC70">
         <v>2</v>
       </c>
+      <c r="AD70">
+        <v>2</v>
+      </c>
+      <c r="AE70">
+        <v>2</v>
+      </c>
     </row>
-    <row r="71" spans="1:29">
+    <row r="71" spans="1:31">
       <c r="B71" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C71">
         <v>50.5039</v>
@@ -6959,13 +7385,19 @@
       <c r="AC71">
         <v>1</v>
       </c>
+      <c r="AD71">
+        <v>1</v>
+      </c>
+      <c r="AE71">
+        <v>1</v>
+      </c>
     </row>
-    <row r="72" spans="1:29">
+    <row r="72" spans="1:31">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B72" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C72">
         <v>43.0731</v>
@@ -7048,13 +7480,19 @@
       <c r="AC72">
         <v>1</v>
       </c>
+      <c r="AD72">
+        <v>1</v>
+      </c>
+      <c r="AE72">
+        <v>1</v>
+      </c>
     </row>
-    <row r="73" spans="1:29">
+    <row r="73" spans="1:31">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B73" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C73">
         <v>35.4437</v>
@@ -7137,13 +7575,19 @@
       <c r="AC73">
         <v>285</v>
       </c>
+      <c r="AD73">
+        <v>355</v>
+      </c>
+      <c r="AE73">
+        <v>454</v>
+      </c>
     </row>
-    <row r="74" spans="1:29">
+    <row r="74" spans="1:31">
       <c r="A74" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B74" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C74">
         <v>32.7157</v>
@@ -7226,13 +7670,19 @@
       <c r="AC74">
         <v>2</v>
       </c>
+      <c r="AD74">
+        <v>2</v>
+      </c>
+      <c r="AE74">
+        <v>2</v>
+      </c>
     </row>
-    <row r="75" spans="1:29">
+    <row r="75" spans="1:31">
       <c r="A75" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B75" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C75">
         <v>29.4241</v>
@@ -7315,10 +7765,16 @@
       <c r="AC75">
         <v>1</v>
       </c>
+      <c r="AD75">
+        <v>1</v>
+      </c>
+      <c r="AE75">
+        <v>1</v>
+      </c>
     </row>
-    <row r="76" spans="1:29">
+    <row r="76" spans="1:31">
       <c r="B76" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C76">
         <v>26.8206</v>
@@ -7399,6 +7855,12 @@
         <v>1</v>
       </c>
       <c r="AC76">
+        <v>1</v>
+      </c>
+      <c r="AD76">
+        <v>1</v>
+      </c>
+      <c r="AE76">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update charts, check if everything still works
</commit_message>
<xml_diff>
--- a/COVID19-Confirmed.xlsx
+++ b/COVID19-Confirmed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="125">
   <si>
     <t>Province/State</t>
   </si>
@@ -109,6 +109,18 @@
     <t>2/17/20</t>
   </si>
   <si>
+    <t>2/18/20</t>
+  </si>
+  <si>
+    <t>2/19/20</t>
+  </si>
+  <si>
+    <t>2/20/20</t>
+  </si>
+  <si>
+    <t>2/21/20</t>
+  </si>
+  <si>
     <t>Anhui</t>
   </si>
   <si>
@@ -268,6 +280,27 @@
     <t>San Antonio, TX</t>
   </si>
   <si>
+    <t>Ashland, NE</t>
+  </si>
+  <si>
+    <t>Travis, CA</t>
+  </si>
+  <si>
+    <t>From Diamond Princess</t>
+  </si>
+  <si>
+    <t>Lackland, TX</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Humboldt County, CA</t>
+  </si>
+  <si>
+    <t>Sacramento County, CA</t>
+  </si>
+  <si>
     <t>Mainland China</t>
   </si>
   <si>
@@ -347,6 +380,15 @@
   </si>
   <si>
     <t>Egypt</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
   </si>
 </sst>
 </file>
@@ -704,13 +746,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE76"/>
+  <dimension ref="A1:AI85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -804,13 +846,25 @@
       <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:35">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C2">
         <v>31.82571</v>
@@ -899,13 +953,25 @@
       <c r="AE2">
         <v>973</v>
       </c>
+      <c r="AF2">
+        <v>982</v>
+      </c>
+      <c r="AG2">
+        <v>986</v>
+      </c>
+      <c r="AH2">
+        <v>987</v>
+      </c>
+      <c r="AI2">
+        <v>988</v>
+      </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:35">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C3">
         <v>40.18238</v>
@@ -994,13 +1060,25 @@
       <c r="AE3">
         <v>381</v>
       </c>
+      <c r="AF3">
+        <v>387</v>
+      </c>
+      <c r="AG3">
+        <v>393</v>
+      </c>
+      <c r="AH3">
+        <v>395</v>
+      </c>
+      <c r="AI3">
+        <v>396</v>
+      </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:35">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C4">
         <v>30.05718</v>
@@ -1089,13 +1167,25 @@
       <c r="AE4">
         <v>553</v>
       </c>
+      <c r="AF4">
+        <v>555</v>
+      </c>
+      <c r="AG4">
+        <v>560</v>
+      </c>
+      <c r="AH4">
+        <v>567</v>
+      </c>
+      <c r="AI4">
+        <v>572</v>
+      </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:35">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C5">
         <v>26.07783</v>
@@ -1184,13 +1274,25 @@
       <c r="AE5">
         <v>290</v>
       </c>
+      <c r="AF5">
+        <v>292</v>
+      </c>
+      <c r="AG5">
+        <v>293</v>
+      </c>
+      <c r="AH5">
+        <v>293</v>
+      </c>
+      <c r="AI5">
+        <v>293</v>
+      </c>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:35">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C6">
         <v>36.0611</v>
@@ -1279,13 +1381,25 @@
       <c r="AE6">
         <v>91</v>
       </c>
+      <c r="AF6">
+        <v>91</v>
+      </c>
+      <c r="AG6">
+        <v>91</v>
+      </c>
+      <c r="AH6">
+        <v>91</v>
+      </c>
+      <c r="AI6">
+        <v>91</v>
+      </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:35">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C7">
         <v>23.33841</v>
@@ -1374,13 +1488,25 @@
       <c r="AE7">
         <v>1322</v>
       </c>
+      <c r="AF7">
+        <v>1328</v>
+      </c>
+      <c r="AG7">
+        <v>1331</v>
+      </c>
+      <c r="AH7">
+        <v>1332</v>
+      </c>
+      <c r="AI7">
+        <v>1333</v>
+      </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:35">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C8">
         <v>23.82908</v>
@@ -1469,13 +1595,25 @@
       <c r="AE8">
         <v>238</v>
       </c>
+      <c r="AF8">
+        <v>242</v>
+      </c>
+      <c r="AG8">
+        <v>244</v>
+      </c>
+      <c r="AH8">
+        <v>245</v>
+      </c>
+      <c r="AI8">
+        <v>246</v>
+      </c>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:35">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C9">
         <v>26.81536</v>
@@ -1564,13 +1702,25 @@
       <c r="AE9">
         <v>146</v>
       </c>
+      <c r="AF9">
+        <v>146</v>
+      </c>
+      <c r="AG9">
+        <v>146</v>
+      </c>
+      <c r="AH9">
+        <v>146</v>
+      </c>
+      <c r="AI9">
+        <v>146</v>
+      </c>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:35">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C10">
         <v>19.19673</v>
@@ -1659,13 +1809,25 @@
       <c r="AE10">
         <v>163</v>
       </c>
+      <c r="AF10">
+        <v>163</v>
+      </c>
+      <c r="AG10">
+        <v>168</v>
+      </c>
+      <c r="AH10">
+        <v>168</v>
+      </c>
+      <c r="AI10">
+        <v>168</v>
+      </c>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:35">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C11">
         <v>38.0428</v>
@@ -1754,13 +1916,25 @@
       <c r="AE11">
         <v>301</v>
       </c>
+      <c r="AF11">
+        <v>306</v>
+      </c>
+      <c r="AG11">
+        <v>306</v>
+      </c>
+      <c r="AH11">
+        <v>307</v>
+      </c>
+      <c r="AI11">
+        <v>308</v>
+      </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:35">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C12">
         <v>47.86199999999999</v>
@@ -1849,13 +2023,25 @@
       <c r="AE12">
         <v>457</v>
       </c>
+      <c r="AF12">
+        <v>464</v>
+      </c>
+      <c r="AG12">
+        <v>470</v>
+      </c>
+      <c r="AH12">
+        <v>476</v>
+      </c>
+      <c r="AI12">
+        <v>479</v>
+      </c>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:35">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C13">
         <v>33.88202</v>
@@ -1944,13 +2130,25 @@
       <c r="AE13">
         <v>1246</v>
       </c>
+      <c r="AF13">
+        <v>1257</v>
+      </c>
+      <c r="AG13">
+        <v>1262</v>
+      </c>
+      <c r="AH13">
+        <v>1265</v>
+      </c>
+      <c r="AI13">
+        <v>1267</v>
+      </c>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:35">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C14">
         <v>30.97564</v>
@@ -2039,13 +2237,25 @@
       <c r="AE14">
         <v>59989</v>
       </c>
+      <c r="AF14">
+        <v>61682</v>
+      </c>
+      <c r="AG14">
+        <v>62031</v>
+      </c>
+      <c r="AH14">
+        <v>62442</v>
+      </c>
+      <c r="AI14">
+        <v>62662</v>
+      </c>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:35">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C15">
         <v>27.61041</v>
@@ -2134,13 +2344,25 @@
       <c r="AE15">
         <v>1006</v>
       </c>
+      <c r="AF15">
+        <v>1007</v>
+      </c>
+      <c r="AG15">
+        <v>1008</v>
+      </c>
+      <c r="AH15">
+        <v>1010</v>
+      </c>
+      <c r="AI15">
+        <v>1011</v>
+      </c>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:35">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C16">
         <v>44.09448</v>
@@ -2229,13 +2451,25 @@
       <c r="AE16">
         <v>72</v>
       </c>
+      <c r="AF16">
+        <v>73</v>
+      </c>
+      <c r="AG16">
+        <v>75</v>
+      </c>
+      <c r="AH16">
+        <v>75</v>
+      </c>
+      <c r="AI16">
+        <v>75</v>
+      </c>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:35">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C17">
         <v>32.97027</v>
@@ -2324,13 +2558,25 @@
       <c r="AE17">
         <v>626</v>
       </c>
+      <c r="AF17">
+        <v>629</v>
+      </c>
+      <c r="AG17">
+        <v>631</v>
+      </c>
+      <c r="AH17">
+        <v>631</v>
+      </c>
+      <c r="AI17">
+        <v>631</v>
+      </c>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:35">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C18">
         <v>27.61401</v>
@@ -2419,13 +2665,25 @@
       <c r="AE18">
         <v>930</v>
       </c>
+      <c r="AF18">
+        <v>933</v>
+      </c>
+      <c r="AG18">
+        <v>934</v>
+      </c>
+      <c r="AH18">
+        <v>934</v>
+      </c>
+      <c r="AI18">
+        <v>934</v>
+      </c>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:35">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C19">
         <v>43.66657</v>
@@ -2514,13 +2772,25 @@
       <c r="AE19">
         <v>89</v>
       </c>
+      <c r="AF19">
+        <v>89</v>
+      </c>
+      <c r="AG19">
+        <v>90</v>
+      </c>
+      <c r="AH19">
+        <v>91</v>
+      </c>
+      <c r="AI19">
+        <v>91</v>
+      </c>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:35">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C20">
         <v>41.29284000000001</v>
@@ -2609,13 +2879,25 @@
       <c r="AE20">
         <v>121</v>
       </c>
+      <c r="AF20">
+        <v>121</v>
+      </c>
+      <c r="AG20">
+        <v>121</v>
+      </c>
+      <c r="AH20">
+        <v>121</v>
+      </c>
+      <c r="AI20">
+        <v>121</v>
+      </c>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:35">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C21">
         <v>37.26923</v>
@@ -2704,13 +2986,25 @@
       <c r="AE21">
         <v>70</v>
       </c>
+      <c r="AF21">
+        <v>70</v>
+      </c>
+      <c r="AG21">
+        <v>71</v>
+      </c>
+      <c r="AH21">
+        <v>71</v>
+      </c>
+      <c r="AI21">
+        <v>71</v>
+      </c>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:35">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C22">
         <v>35.65945</v>
@@ -2799,13 +3093,25 @@
       <c r="AE22">
         <v>18</v>
       </c>
+      <c r="AF22">
+        <v>18</v>
+      </c>
+      <c r="AG22">
+        <v>18</v>
+      </c>
+      <c r="AH22">
+        <v>18</v>
+      </c>
+      <c r="AI22">
+        <v>18</v>
+      </c>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:35">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C23">
         <v>35.19165</v>
@@ -2894,13 +3200,25 @@
       <c r="AE23">
         <v>240</v>
       </c>
+      <c r="AF23">
+        <v>240</v>
+      </c>
+      <c r="AG23">
+        <v>242</v>
+      </c>
+      <c r="AH23">
+        <v>245</v>
+      </c>
+      <c r="AI23">
+        <v>245</v>
+      </c>
     </row>
-    <row r="24" spans="1:31">
+    <row r="24" spans="1:35">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C24">
         <v>36.34377</v>
@@ -2989,13 +3307,25 @@
       <c r="AE24">
         <v>541</v>
       </c>
+      <c r="AF24">
+        <v>543</v>
+      </c>
+      <c r="AG24">
+        <v>544</v>
+      </c>
+      <c r="AH24">
+        <v>546</v>
+      </c>
+      <c r="AI24">
+        <v>749</v>
+      </c>
     </row>
-    <row r="25" spans="1:31">
+    <row r="25" spans="1:35">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C25">
         <v>31.20327</v>
@@ -3084,13 +3414,25 @@
       <c r="AE25">
         <v>333</v>
       </c>
+      <c r="AF25">
+        <v>333</v>
+      </c>
+      <c r="AG25">
+        <v>333</v>
+      </c>
+      <c r="AH25">
+        <v>334</v>
+      </c>
+      <c r="AI25">
+        <v>334</v>
+      </c>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:35">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C26">
         <v>37.57769</v>
@@ -3179,13 +3521,25 @@
       <c r="AE26">
         <v>130</v>
       </c>
+      <c r="AF26">
+        <v>131</v>
+      </c>
+      <c r="AG26">
+        <v>131</v>
+      </c>
+      <c r="AH26">
+        <v>132</v>
+      </c>
+      <c r="AI26">
+        <v>132</v>
+      </c>
     </row>
-    <row r="27" spans="1:31">
+    <row r="27" spans="1:35">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C27">
         <v>30.61714</v>
@@ -3274,13 +3628,25 @@
       <c r="AE27">
         <v>495</v>
       </c>
+      <c r="AF27">
+        <v>508</v>
+      </c>
+      <c r="AG27">
+        <v>514</v>
+      </c>
+      <c r="AH27">
+        <v>520</v>
+      </c>
+      <c r="AI27">
+        <v>525</v>
+      </c>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:35">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C28">
         <v>39.29362</v>
@@ -3369,13 +3735,25 @@
       <c r="AE28">
         <v>125</v>
       </c>
+      <c r="AF28">
+        <v>128</v>
+      </c>
+      <c r="AG28">
+        <v>130</v>
+      </c>
+      <c r="AH28">
+        <v>131</v>
+      </c>
+      <c r="AI28">
+        <v>132</v>
+      </c>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:35">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C29">
         <v>30.1534</v>
@@ -3464,13 +3842,25 @@
       <c r="AE29">
         <v>1</v>
       </c>
+      <c r="AF29">
+        <v>1</v>
+      </c>
+      <c r="AG29">
+        <v>1</v>
+      </c>
+      <c r="AH29">
+        <v>1</v>
+      </c>
+      <c r="AI29">
+        <v>1</v>
+      </c>
     </row>
-    <row r="30" spans="1:31">
+    <row r="30" spans="1:35">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C30">
         <v>41.11981</v>
@@ -3559,13 +3949,25 @@
       <c r="AE30">
         <v>75</v>
       </c>
+      <c r="AF30">
+        <v>76</v>
+      </c>
+      <c r="AG30">
+        <v>76</v>
+      </c>
+      <c r="AH30">
+        <v>76</v>
+      </c>
+      <c r="AI30">
+        <v>76</v>
+      </c>
     </row>
-    <row r="31" spans="1:31">
+    <row r="31" spans="1:35">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C31">
         <v>24.97411</v>
@@ -3654,13 +4056,25 @@
       <c r="AE31">
         <v>171</v>
       </c>
+      <c r="AF31">
+        <v>172</v>
+      </c>
+      <c r="AG31">
+        <v>172</v>
+      </c>
+      <c r="AH31">
+        <v>174</v>
+      </c>
+      <c r="AI31">
+        <v>174</v>
+      </c>
     </row>
-    <row r="32" spans="1:31">
+    <row r="32" spans="1:35">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C32">
         <v>29.18251</v>
@@ -3749,10 +4163,22 @@
       <c r="AE32">
         <v>1171</v>
       </c>
+      <c r="AF32">
+        <v>1172</v>
+      </c>
+      <c r="AG32">
+        <v>1174</v>
+      </c>
+      <c r="AH32">
+        <v>1175</v>
+      </c>
+      <c r="AI32">
+        <v>1203</v>
+      </c>
     </row>
-    <row r="33" spans="1:31">
+    <row r="33" spans="1:35">
       <c r="B33" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="C33">
         <v>13.7563</v>
@@ -3841,10 +4267,22 @@
       <c r="AE33">
         <v>35</v>
       </c>
+      <c r="AF33">
+        <v>35</v>
+      </c>
+      <c r="AG33">
+        <v>35</v>
+      </c>
+      <c r="AH33">
+        <v>35</v>
+      </c>
+      <c r="AI33">
+        <v>35</v>
+      </c>
     </row>
-    <row r="34" spans="1:31">
+    <row r="34" spans="1:35">
       <c r="B34" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C34">
         <v>35.6762</v>
@@ -3933,10 +4371,22 @@
       <c r="AE34">
         <v>66</v>
       </c>
+      <c r="AF34">
+        <v>74</v>
+      </c>
+      <c r="AG34">
+        <v>84</v>
+      </c>
+      <c r="AH34">
+        <v>94</v>
+      </c>
+      <c r="AI34">
+        <v>105</v>
+      </c>
     </row>
-    <row r="35" spans="1:31">
+    <row r="35" spans="1:35">
       <c r="B35" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C35">
         <v>37.5665</v>
@@ -4025,13 +4475,25 @@
       <c r="AE35">
         <v>30</v>
       </c>
+      <c r="AF35">
+        <v>31</v>
+      </c>
+      <c r="AG35">
+        <v>31</v>
+      </c>
+      <c r="AH35">
+        <v>104</v>
+      </c>
+      <c r="AI35">
+        <v>204</v>
+      </c>
     </row>
-    <row r="36" spans="1:31">
+    <row r="36" spans="1:35">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C36">
         <v>23.6978</v>
@@ -4120,13 +4582,25 @@
       <c r="AE36">
         <v>22</v>
       </c>
+      <c r="AF36">
+        <v>22</v>
+      </c>
+      <c r="AG36">
+        <v>23</v>
+      </c>
+      <c r="AH36">
+        <v>24</v>
+      </c>
+      <c r="AI36">
+        <v>26</v>
+      </c>
     </row>
-    <row r="37" spans="1:31">
+    <row r="37" spans="1:35">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C37">
         <v>47.7511</v>
@@ -4215,13 +4689,25 @@
       <c r="AE37">
         <v>1</v>
       </c>
+      <c r="AF37">
+        <v>1</v>
+      </c>
+      <c r="AG37">
+        <v>1</v>
+      </c>
+      <c r="AH37">
+        <v>1</v>
+      </c>
+      <c r="AI37">
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="1:31">
+    <row r="38" spans="1:35">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C38">
         <v>40.6331</v>
@@ -4310,13 +4796,25 @@
       <c r="AE38">
         <v>2</v>
       </c>
+      <c r="AF38">
+        <v>2</v>
+      </c>
+      <c r="AG38">
+        <v>2</v>
+      </c>
+      <c r="AH38">
+        <v>2</v>
+      </c>
+      <c r="AI38">
+        <v>2</v>
+      </c>
     </row>
-    <row r="39" spans="1:31">
+    <row r="39" spans="1:35">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C39">
         <v>34.0489</v>
@@ -4405,13 +4903,25 @@
       <c r="AE39">
         <v>1</v>
       </c>
+      <c r="AF39">
+        <v>1</v>
+      </c>
+      <c r="AG39">
+        <v>1</v>
+      </c>
+      <c r="AH39">
+        <v>1</v>
+      </c>
+      <c r="AI39">
+        <v>1</v>
+      </c>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:35">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C40">
         <v>22.1987</v>
@@ -4500,13 +5010,25 @@
       <c r="AE40">
         <v>10</v>
       </c>
+      <c r="AF40">
+        <v>10</v>
+      </c>
+      <c r="AG40">
+        <v>10</v>
+      </c>
+      <c r="AH40">
+        <v>10</v>
+      </c>
+      <c r="AI40">
+        <v>10</v>
+      </c>
     </row>
-    <row r="41" spans="1:31">
+    <row r="41" spans="1:35">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C41">
         <v>22.3193</v>
@@ -4595,10 +5117,22 @@
       <c r="AE41">
         <v>60</v>
       </c>
+      <c r="AF41">
+        <v>62</v>
+      </c>
+      <c r="AG41">
+        <v>63</v>
+      </c>
+      <c r="AH41">
+        <v>68</v>
+      </c>
+      <c r="AI41">
+        <v>68</v>
+      </c>
     </row>
-    <row r="42" spans="1:31">
+    <row r="42" spans="1:35">
       <c r="B42" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="C42">
         <v>1.3521</v>
@@ -4687,10 +5221,22 @@
       <c r="AE42">
         <v>77</v>
       </c>
+      <c r="AF42">
+        <v>81</v>
+      </c>
+      <c r="AG42">
+        <v>84</v>
+      </c>
+      <c r="AH42">
+        <v>84</v>
+      </c>
+      <c r="AI42">
+        <v>85</v>
+      </c>
     </row>
-    <row r="43" spans="1:31">
+    <row r="43" spans="1:35">
       <c r="B43" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="C43">
         <v>21.0278</v>
@@ -4779,10 +5325,22 @@
       <c r="AE43">
         <v>16</v>
       </c>
+      <c r="AF43">
+        <v>16</v>
+      </c>
+      <c r="AG43">
+        <v>16</v>
+      </c>
+      <c r="AH43">
+        <v>16</v>
+      </c>
+      <c r="AI43">
+        <v>16</v>
+      </c>
     </row>
-    <row r="44" spans="1:31">
+    <row r="44" spans="1:35">
       <c r="B44" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="C44">
         <v>46.2276</v>
@@ -4871,10 +5429,22 @@
       <c r="AE44">
         <v>12</v>
       </c>
+      <c r="AF44">
+        <v>12</v>
+      </c>
+      <c r="AG44">
+        <v>12</v>
+      </c>
+      <c r="AH44">
+        <v>12</v>
+      </c>
+      <c r="AI44">
+        <v>12</v>
+      </c>
     </row>
-    <row r="45" spans="1:31">
+    <row r="45" spans="1:35">
       <c r="B45" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="C45">
         <v>28.3949</v>
@@ -4963,10 +5533,22 @@
       <c r="AE45">
         <v>1</v>
       </c>
+      <c r="AF45">
+        <v>1</v>
+      </c>
+      <c r="AG45">
+        <v>1</v>
+      </c>
+      <c r="AH45">
+        <v>1</v>
+      </c>
+      <c r="AI45">
+        <v>1</v>
+      </c>
     </row>
-    <row r="46" spans="1:31">
+    <row r="46" spans="1:35">
       <c r="B46" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="C46">
         <v>4.2105</v>
@@ -5055,13 +5637,25 @@
       <c r="AE46">
         <v>22</v>
       </c>
+      <c r="AF46">
+        <v>22</v>
+      </c>
+      <c r="AG46">
+        <v>22</v>
+      </c>
+      <c r="AH46">
+        <v>22</v>
+      </c>
+      <c r="AI46">
+        <v>22</v>
+      </c>
     </row>
-    <row r="47" spans="1:31">
+    <row r="47" spans="1:35">
       <c r="A47" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C47">
         <v>43.6532</v>
@@ -5150,13 +5744,25 @@
       <c r="AE47">
         <v>2</v>
       </c>
+      <c r="AF47">
+        <v>2</v>
+      </c>
+      <c r="AG47">
+        <v>2</v>
+      </c>
+      <c r="AH47">
+        <v>2</v>
+      </c>
+      <c r="AI47">
+        <v>2</v>
+      </c>
     </row>
-    <row r="48" spans="1:31">
+    <row r="48" spans="1:35">
       <c r="A48" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C48">
         <v>49.2827</v>
@@ -5245,13 +5851,25 @@
       <c r="AE48">
         <v>5</v>
       </c>
+      <c r="AF48">
+        <v>5</v>
+      </c>
+      <c r="AG48">
+        <v>5</v>
+      </c>
+      <c r="AH48">
+        <v>5</v>
+      </c>
+      <c r="AI48">
+        <v>6</v>
+      </c>
     </row>
-    <row r="49" spans="1:31">
+    <row r="49" spans="1:35">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C49">
         <v>33.7879</v>
@@ -5340,13 +5958,25 @@
       <c r="AE49">
         <v>1</v>
       </c>
+      <c r="AF49">
+        <v>1</v>
+      </c>
+      <c r="AG49">
+        <v>1</v>
+      </c>
+      <c r="AH49">
+        <v>1</v>
+      </c>
+      <c r="AI49">
+        <v>1</v>
+      </c>
     </row>
-    <row r="50" spans="1:31">
+    <row r="50" spans="1:35">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C50">
         <v>34.0522</v>
@@ -5435,13 +6065,25 @@
       <c r="AE50">
         <v>1</v>
       </c>
+      <c r="AF50">
+        <v>1</v>
+      </c>
+      <c r="AG50">
+        <v>1</v>
+      </c>
+      <c r="AH50">
+        <v>1</v>
+      </c>
+      <c r="AI50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="1:31">
+    <row r="51" spans="1:35">
       <c r="A51" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B51" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="C51">
         <v>-33.8688</v>
@@ -5530,13 +6172,25 @@
       <c r="AE51">
         <v>4</v>
       </c>
+      <c r="AF51">
+        <v>4</v>
+      </c>
+      <c r="AG51">
+        <v>4</v>
+      </c>
+      <c r="AH51">
+        <v>4</v>
+      </c>
+      <c r="AI51">
+        <v>4</v>
+      </c>
     </row>
-    <row r="52" spans="1:31">
+    <row r="52" spans="1:35">
       <c r="A52" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B52" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="C52">
         <v>-37.8136</v>
@@ -5625,13 +6279,25 @@
       <c r="AE52">
         <v>4</v>
       </c>
+      <c r="AF52">
+        <v>4</v>
+      </c>
+      <c r="AG52">
+        <v>4</v>
+      </c>
+      <c r="AH52">
+        <v>4</v>
+      </c>
+      <c r="AI52">
+        <v>4</v>
+      </c>
     </row>
-    <row r="53" spans="1:31">
+    <row r="53" spans="1:35">
       <c r="A53" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="C53">
         <v>-27.4698</v>
@@ -5720,10 +6386,22 @@
       <c r="AE53">
         <v>5</v>
       </c>
+      <c r="AF53">
+        <v>5</v>
+      </c>
+      <c r="AG53">
+        <v>5</v>
+      </c>
+      <c r="AH53">
+        <v>5</v>
+      </c>
+      <c r="AI53">
+        <v>5</v>
+      </c>
     </row>
-    <row r="54" spans="1:31">
+    <row r="54" spans="1:35">
       <c r="B54" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="C54">
         <v>12.5657</v>
@@ -5812,10 +6490,22 @@
       <c r="AE54">
         <v>1</v>
       </c>
+      <c r="AF54">
+        <v>1</v>
+      </c>
+      <c r="AG54">
+        <v>1</v>
+      </c>
+      <c r="AH54">
+        <v>1</v>
+      </c>
+      <c r="AI54">
+        <v>1</v>
+      </c>
     </row>
-    <row r="55" spans="1:31">
+    <row r="55" spans="1:35">
       <c r="B55" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="C55">
         <v>7.8731</v>
@@ -5904,10 +6594,22 @@
       <c r="AE55">
         <v>1</v>
       </c>
+      <c r="AF55">
+        <v>1</v>
+      </c>
+      <c r="AG55">
+        <v>1</v>
+      </c>
+      <c r="AH55">
+        <v>1</v>
+      </c>
+      <c r="AI55">
+        <v>1</v>
+      </c>
     </row>
-    <row r="56" spans="1:31">
+    <row r="56" spans="1:35">
       <c r="B56" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="C56">
         <v>51.1657</v>
@@ -5996,10 +6698,22 @@
       <c r="AE56">
         <v>16</v>
       </c>
+      <c r="AF56">
+        <v>16</v>
+      </c>
+      <c r="AG56">
+        <v>16</v>
+      </c>
+      <c r="AH56">
+        <v>16</v>
+      </c>
+      <c r="AI56">
+        <v>16</v>
+      </c>
     </row>
-    <row r="57" spans="1:31">
+    <row r="57" spans="1:35">
       <c r="B57" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="C57">
         <v>61.9241</v>
@@ -6088,10 +6802,22 @@
       <c r="AE57">
         <v>1</v>
       </c>
+      <c r="AF57">
+        <v>1</v>
+      </c>
+      <c r="AG57">
+        <v>1</v>
+      </c>
+      <c r="AH57">
+        <v>1</v>
+      </c>
+      <c r="AI57">
+        <v>1</v>
+      </c>
     </row>
-    <row r="58" spans="1:31">
+    <row r="58" spans="1:35">
       <c r="B58" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="C58">
         <v>23.4241</v>
@@ -6180,10 +6906,22 @@
       <c r="AE58">
         <v>9</v>
       </c>
+      <c r="AF58">
+        <v>9</v>
+      </c>
+      <c r="AG58">
+        <v>9</v>
+      </c>
+      <c r="AH58">
+        <v>9</v>
+      </c>
+      <c r="AI58">
+        <v>9</v>
+      </c>
     </row>
-    <row r="59" spans="1:31">
+    <row r="59" spans="1:35">
       <c r="B59" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="C59">
         <v>12.8797</v>
@@ -6272,10 +7010,22 @@
       <c r="AE59">
         <v>3</v>
       </c>
+      <c r="AF59">
+        <v>3</v>
+      </c>
+      <c r="AG59">
+        <v>3</v>
+      </c>
+      <c r="AH59">
+        <v>3</v>
+      </c>
+      <c r="AI59">
+        <v>3</v>
+      </c>
     </row>
-    <row r="60" spans="1:31">
+    <row r="60" spans="1:35">
       <c r="B60" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="C60">
         <v>20.5937</v>
@@ -6364,13 +7114,25 @@
       <c r="AE60">
         <v>3</v>
       </c>
+      <c r="AF60">
+        <v>3</v>
+      </c>
+      <c r="AG60">
+        <v>3</v>
+      </c>
+      <c r="AH60">
+        <v>3</v>
+      </c>
+      <c r="AI60">
+        <v>3</v>
+      </c>
     </row>
-    <row r="61" spans="1:31">
+    <row r="61" spans="1:35">
       <c r="A61" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B61" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C61">
         <v>42.9849</v>
@@ -6459,10 +7221,22 @@
       <c r="AE61">
         <v>1</v>
       </c>
+      <c r="AF61">
+        <v>1</v>
+      </c>
+      <c r="AG61">
+        <v>1</v>
+      </c>
+      <c r="AH61">
+        <v>1</v>
+      </c>
+      <c r="AI61">
+        <v>1</v>
+      </c>
     </row>
-    <row r="62" spans="1:31">
+    <row r="62" spans="1:35">
       <c r="B62" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="C62">
         <v>41.8719</v>
@@ -6551,10 +7325,22 @@
       <c r="AE62">
         <v>3</v>
       </c>
+      <c r="AF62">
+        <v>3</v>
+      </c>
+      <c r="AG62">
+        <v>3</v>
+      </c>
+      <c r="AH62">
+        <v>3</v>
+      </c>
+      <c r="AI62">
+        <v>20</v>
+      </c>
     </row>
-    <row r="63" spans="1:31">
+    <row r="63" spans="1:35">
       <c r="B63" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="C63">
         <v>55.3781</v>
@@ -6643,10 +7429,22 @@
       <c r="AE63">
         <v>9</v>
       </c>
+      <c r="AF63">
+        <v>9</v>
+      </c>
+      <c r="AG63">
+        <v>9</v>
+      </c>
+      <c r="AH63">
+        <v>9</v>
+      </c>
+      <c r="AI63">
+        <v>9</v>
+      </c>
     </row>
-    <row r="64" spans="1:31">
+    <row r="64" spans="1:35">
       <c r="B64" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="C64">
         <v>61.52399999999999</v>
@@ -6735,10 +7533,22 @@
       <c r="AE64">
         <v>2</v>
       </c>
+      <c r="AF64">
+        <v>2</v>
+      </c>
+      <c r="AG64">
+        <v>2</v>
+      </c>
+      <c r="AH64">
+        <v>2</v>
+      </c>
+      <c r="AI64">
+        <v>2</v>
+      </c>
     </row>
-    <row r="65" spans="1:31">
+    <row r="65" spans="1:35">
       <c r="B65" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="C65">
         <v>60.1282</v>
@@ -6827,13 +7637,25 @@
       <c r="AE65">
         <v>1</v>
       </c>
+      <c r="AF65">
+        <v>1</v>
+      </c>
+      <c r="AG65">
+        <v>1</v>
+      </c>
+      <c r="AH65">
+        <v>1</v>
+      </c>
+      <c r="AI65">
+        <v>1</v>
+      </c>
     </row>
-    <row r="66" spans="1:31">
+    <row r="66" spans="1:35">
       <c r="A66" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B66" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C66">
         <v>37.3541</v>
@@ -6922,10 +7744,22 @@
       <c r="AE66">
         <v>2</v>
       </c>
+      <c r="AF66">
+        <v>2</v>
+      </c>
+      <c r="AG66">
+        <v>2</v>
+      </c>
+      <c r="AH66">
+        <v>2</v>
+      </c>
+      <c r="AI66">
+        <v>2</v>
+      </c>
     </row>
-    <row r="67" spans="1:31">
+    <row r="67" spans="1:35">
       <c r="B67" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="C67">
         <v>40.4637</v>
@@ -7014,13 +7848,25 @@
       <c r="AE67">
         <v>2</v>
       </c>
+      <c r="AF67">
+        <v>2</v>
+      </c>
+      <c r="AG67">
+        <v>2</v>
+      </c>
+      <c r="AH67">
+        <v>2</v>
+      </c>
+      <c r="AI67">
+        <v>2</v>
+      </c>
     </row>
-    <row r="68" spans="1:31">
+    <row r="68" spans="1:35">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B68" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="C68">
         <v>-34.9285</v>
@@ -7109,13 +7955,25 @@
       <c r="AE68">
         <v>2</v>
       </c>
+      <c r="AF68">
+        <v>2</v>
+      </c>
+      <c r="AG68">
+        <v>2</v>
+      </c>
+      <c r="AH68">
+        <v>2</v>
+      </c>
+      <c r="AI68">
+        <v>2</v>
+      </c>
     </row>
-    <row r="69" spans="1:31">
+    <row r="69" spans="1:35">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B69" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C69">
         <v>42.3601</v>
@@ -7204,13 +8062,25 @@
       <c r="AE69">
         <v>1</v>
       </c>
+      <c r="AF69">
+        <v>1</v>
+      </c>
+      <c r="AG69">
+        <v>1</v>
+      </c>
+      <c r="AH69">
+        <v>1</v>
+      </c>
+      <c r="AI69">
+        <v>1</v>
+      </c>
     </row>
-    <row r="70" spans="1:31">
+    <row r="70" spans="1:35">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B70" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C70">
         <v>36.5761</v>
@@ -7299,10 +8169,22 @@
       <c r="AE70">
         <v>2</v>
       </c>
+      <c r="AF70">
+        <v>2</v>
+      </c>
+      <c r="AG70">
+        <v>2</v>
+      </c>
+      <c r="AH70">
+        <v>2</v>
+      </c>
+      <c r="AI70">
+        <v>2</v>
+      </c>
     </row>
-    <row r="71" spans="1:31">
+    <row r="71" spans="1:35">
       <c r="B71" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="C71">
         <v>50.5039</v>
@@ -7391,13 +8273,25 @@
       <c r="AE71">
         <v>1</v>
       </c>
+      <c r="AF71">
+        <v>1</v>
+      </c>
+      <c r="AG71">
+        <v>1</v>
+      </c>
+      <c r="AH71">
+        <v>1</v>
+      </c>
+      <c r="AI71">
+        <v>1</v>
+      </c>
     </row>
-    <row r="72" spans="1:31">
+    <row r="72" spans="1:35">
       <c r="A72" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B72" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C72">
         <v>43.0731</v>
@@ -7486,19 +8380,31 @@
       <c r="AE72">
         <v>1</v>
       </c>
+      <c r="AF72">
+        <v>1</v>
+      </c>
+      <c r="AG72">
+        <v>1</v>
+      </c>
+      <c r="AH72">
+        <v>1</v>
+      </c>
+      <c r="AI72">
+        <v>1</v>
+      </c>
     </row>
-    <row r="73" spans="1:31">
+    <row r="73" spans="1:35">
       <c r="A73" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B73" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C73">
         <v>35.4437</v>
       </c>
       <c r="D73">
-        <v>129.638</v>
+        <v>139.638</v>
       </c>
       <c r="E73">
         <v>0</v>
@@ -7581,13 +8487,25 @@
       <c r="AE73">
         <v>454</v>
       </c>
+      <c r="AF73">
+        <v>542</v>
+      </c>
+      <c r="AG73">
+        <v>621</v>
+      </c>
+      <c r="AH73">
+        <v>634</v>
+      </c>
+      <c r="AI73">
+        <v>634</v>
+      </c>
     </row>
-    <row r="74" spans="1:31">
+    <row r="74" spans="1:35">
       <c r="A74" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B74" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C74">
         <v>32.7157</v>
@@ -7676,13 +8594,25 @@
       <c r="AE74">
         <v>2</v>
       </c>
+      <c r="AF74">
+        <v>2</v>
+      </c>
+      <c r="AG74">
+        <v>2</v>
+      </c>
+      <c r="AH74">
+        <v>2</v>
+      </c>
+      <c r="AI74">
+        <v>2</v>
+      </c>
     </row>
-    <row r="75" spans="1:31">
+    <row r="75" spans="1:35">
       <c r="A75" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B75" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C75">
         <v>29.4241</v>
@@ -7771,10 +8701,22 @@
       <c r="AE75">
         <v>1</v>
       </c>
+      <c r="AF75">
+        <v>1</v>
+      </c>
+      <c r="AG75">
+        <v>1</v>
+      </c>
+      <c r="AH75">
+        <v>1</v>
+      </c>
+      <c r="AI75">
+        <v>1</v>
+      </c>
     </row>
-    <row r="76" spans="1:31">
+    <row r="76" spans="1:35">
       <c r="B76" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="C76">
         <v>26.8206</v>
@@ -7861,6 +8803,978 @@
         <v>1</v>
       </c>
       <c r="AE76">
+        <v>1</v>
+      </c>
+      <c r="AF76">
+        <v>1</v>
+      </c>
+      <c r="AG76">
+        <v>1</v>
+      </c>
+      <c r="AH76">
+        <v>1</v>
+      </c>
+      <c r="AI76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:35">
+      <c r="B77" t="s">
+        <v>122</v>
+      </c>
+      <c r="C77">
+        <v>32.4279</v>
+      </c>
+      <c r="D77">
+        <v>53.688</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+      <c r="K77">
+        <v>0</v>
+      </c>
+      <c r="L77">
+        <v>0</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="N77">
+        <v>0</v>
+      </c>
+      <c r="O77">
+        <v>0</v>
+      </c>
+      <c r="P77">
+        <v>0</v>
+      </c>
+      <c r="Q77">
+        <v>0</v>
+      </c>
+      <c r="R77">
+        <v>0</v>
+      </c>
+      <c r="S77">
+        <v>0</v>
+      </c>
+      <c r="T77">
+        <v>0</v>
+      </c>
+      <c r="U77">
+        <v>0</v>
+      </c>
+      <c r="V77">
+        <v>0</v>
+      </c>
+      <c r="W77">
+        <v>0</v>
+      </c>
+      <c r="X77">
+        <v>0</v>
+      </c>
+      <c r="Y77">
+        <v>0</v>
+      </c>
+      <c r="Z77">
+        <v>0</v>
+      </c>
+      <c r="AA77">
+        <v>0</v>
+      </c>
+      <c r="AB77">
+        <v>0</v>
+      </c>
+      <c r="AC77">
+        <v>0</v>
+      </c>
+      <c r="AD77">
+        <v>0</v>
+      </c>
+      <c r="AE77">
+        <v>0</v>
+      </c>
+      <c r="AF77">
+        <v>0</v>
+      </c>
+      <c r="AG77">
+        <v>2</v>
+      </c>
+      <c r="AH77">
+        <v>5</v>
+      </c>
+      <c r="AI77">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:35">
+      <c r="A78" t="s">
+        <v>88</v>
+      </c>
+      <c r="B78" t="s">
+        <v>99</v>
+      </c>
+      <c r="C78">
+        <v>41.0652</v>
+      </c>
+      <c r="D78">
+        <v>-96.3339</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78">
+        <v>0</v>
+      </c>
+      <c r="N78">
+        <v>0</v>
+      </c>
+      <c r="O78">
+        <v>0</v>
+      </c>
+      <c r="P78">
+        <v>0</v>
+      </c>
+      <c r="Q78">
+        <v>0</v>
+      </c>
+      <c r="R78">
+        <v>0</v>
+      </c>
+      <c r="S78">
+        <v>0</v>
+      </c>
+      <c r="T78">
+        <v>0</v>
+      </c>
+      <c r="U78">
+        <v>0</v>
+      </c>
+      <c r="V78">
+        <v>0</v>
+      </c>
+      <c r="W78">
+        <v>0</v>
+      </c>
+      <c r="X78">
+        <v>0</v>
+      </c>
+      <c r="Y78">
+        <v>0</v>
+      </c>
+      <c r="Z78">
+        <v>0</v>
+      </c>
+      <c r="AA78">
+        <v>0</v>
+      </c>
+      <c r="AB78">
+        <v>0</v>
+      </c>
+      <c r="AC78">
+        <v>0</v>
+      </c>
+      <c r="AD78">
+        <v>0</v>
+      </c>
+      <c r="AE78">
+        <v>0</v>
+      </c>
+      <c r="AF78">
+        <v>0</v>
+      </c>
+      <c r="AG78">
+        <v>0</v>
+      </c>
+      <c r="AH78">
+        <v>0</v>
+      </c>
+      <c r="AI78">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="1:35">
+      <c r="A79" t="s">
+        <v>89</v>
+      </c>
+      <c r="B79" t="s">
+        <v>99</v>
+      </c>
+      <c r="C79">
+        <v>38.2721</v>
+      </c>
+      <c r="D79">
+        <v>-121.9399</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <v>0</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+      <c r="N79">
+        <v>0</v>
+      </c>
+      <c r="O79">
+        <v>0</v>
+      </c>
+      <c r="P79">
+        <v>0</v>
+      </c>
+      <c r="Q79">
+        <v>0</v>
+      </c>
+      <c r="R79">
+        <v>0</v>
+      </c>
+      <c r="S79">
+        <v>0</v>
+      </c>
+      <c r="T79">
+        <v>0</v>
+      </c>
+      <c r="U79">
+        <v>0</v>
+      </c>
+      <c r="V79">
+        <v>0</v>
+      </c>
+      <c r="W79">
+        <v>0</v>
+      </c>
+      <c r="X79">
+        <v>0</v>
+      </c>
+      <c r="Y79">
+        <v>0</v>
+      </c>
+      <c r="Z79">
+        <v>0</v>
+      </c>
+      <c r="AA79">
+        <v>0</v>
+      </c>
+      <c r="AB79">
+        <v>0</v>
+      </c>
+      <c r="AC79">
+        <v>0</v>
+      </c>
+      <c r="AD79">
+        <v>0</v>
+      </c>
+      <c r="AE79">
+        <v>0</v>
+      </c>
+      <c r="AF79">
+        <v>0</v>
+      </c>
+      <c r="AG79">
+        <v>0</v>
+      </c>
+      <c r="AH79">
+        <v>0</v>
+      </c>
+      <c r="AI79">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:35">
+      <c r="A80" t="s">
+        <v>90</v>
+      </c>
+      <c r="B80" t="s">
+        <v>106</v>
+      </c>
+      <c r="C80">
+        <v>35.4437</v>
+      </c>
+      <c r="D80">
+        <v>139.638</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <v>0</v>
+      </c>
+      <c r="M80">
+        <v>0</v>
+      </c>
+      <c r="N80">
+        <v>0</v>
+      </c>
+      <c r="O80">
+        <v>0</v>
+      </c>
+      <c r="P80">
+        <v>0</v>
+      </c>
+      <c r="Q80">
+        <v>0</v>
+      </c>
+      <c r="R80">
+        <v>0</v>
+      </c>
+      <c r="S80">
+        <v>0</v>
+      </c>
+      <c r="T80">
+        <v>0</v>
+      </c>
+      <c r="U80">
+        <v>0</v>
+      </c>
+      <c r="V80">
+        <v>0</v>
+      </c>
+      <c r="W80">
+        <v>0</v>
+      </c>
+      <c r="X80">
+        <v>0</v>
+      </c>
+      <c r="Y80">
+        <v>0</v>
+      </c>
+      <c r="Z80">
+        <v>0</v>
+      </c>
+      <c r="AA80">
+        <v>0</v>
+      </c>
+      <c r="AB80">
+        <v>0</v>
+      </c>
+      <c r="AC80">
+        <v>0</v>
+      </c>
+      <c r="AD80">
+        <v>0</v>
+      </c>
+      <c r="AE80">
+        <v>0</v>
+      </c>
+      <c r="AF80">
+        <v>0</v>
+      </c>
+      <c r="AG80">
+        <v>0</v>
+      </c>
+      <c r="AH80">
+        <v>0</v>
+      </c>
+      <c r="AI80">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:35">
+      <c r="A81" t="s">
+        <v>91</v>
+      </c>
+      <c r="B81" t="s">
+        <v>99</v>
+      </c>
+      <c r="C81">
+        <v>29.3829</v>
+      </c>
+      <c r="D81">
+        <v>-98.6134</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
+      <c r="L81">
+        <v>0</v>
+      </c>
+      <c r="M81">
+        <v>0</v>
+      </c>
+      <c r="N81">
+        <v>0</v>
+      </c>
+      <c r="O81">
+        <v>0</v>
+      </c>
+      <c r="P81">
+        <v>0</v>
+      </c>
+      <c r="Q81">
+        <v>0</v>
+      </c>
+      <c r="R81">
+        <v>0</v>
+      </c>
+      <c r="S81">
+        <v>0</v>
+      </c>
+      <c r="T81">
+        <v>0</v>
+      </c>
+      <c r="U81">
+        <v>0</v>
+      </c>
+      <c r="V81">
+        <v>0</v>
+      </c>
+      <c r="W81">
+        <v>0</v>
+      </c>
+      <c r="X81">
+        <v>0</v>
+      </c>
+      <c r="Y81">
+        <v>0</v>
+      </c>
+      <c r="Z81">
+        <v>0</v>
+      </c>
+      <c r="AA81">
+        <v>0</v>
+      </c>
+      <c r="AB81">
+        <v>0</v>
+      </c>
+      <c r="AC81">
+        <v>0</v>
+      </c>
+      <c r="AD81">
+        <v>0</v>
+      </c>
+      <c r="AE81">
+        <v>0</v>
+      </c>
+      <c r="AF81">
+        <v>0</v>
+      </c>
+      <c r="AG81">
+        <v>0</v>
+      </c>
+      <c r="AH81">
+        <v>0</v>
+      </c>
+      <c r="AI81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:35">
+      <c r="A82" t="s">
+        <v>90</v>
+      </c>
+      <c r="B82" t="s">
+        <v>123</v>
+      </c>
+      <c r="C82">
+        <v>31.0461</v>
+      </c>
+      <c r="D82">
+        <v>34.8516</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
+      <c r="L82">
+        <v>0</v>
+      </c>
+      <c r="M82">
+        <v>0</v>
+      </c>
+      <c r="N82">
+        <v>0</v>
+      </c>
+      <c r="O82">
+        <v>0</v>
+      </c>
+      <c r="P82">
+        <v>0</v>
+      </c>
+      <c r="Q82">
+        <v>0</v>
+      </c>
+      <c r="R82">
+        <v>0</v>
+      </c>
+      <c r="S82">
+        <v>0</v>
+      </c>
+      <c r="T82">
+        <v>0</v>
+      </c>
+      <c r="U82">
+        <v>0</v>
+      </c>
+      <c r="V82">
+        <v>0</v>
+      </c>
+      <c r="W82">
+        <v>0</v>
+      </c>
+      <c r="X82">
+        <v>0</v>
+      </c>
+      <c r="Y82">
+        <v>0</v>
+      </c>
+      <c r="Z82">
+        <v>0</v>
+      </c>
+      <c r="AA82">
+        <v>0</v>
+      </c>
+      <c r="AB82">
+        <v>0</v>
+      </c>
+      <c r="AC82">
+        <v>0</v>
+      </c>
+      <c r="AD82">
+        <v>0</v>
+      </c>
+      <c r="AE82">
+        <v>0</v>
+      </c>
+      <c r="AF82">
+        <v>0</v>
+      </c>
+      <c r="AG82">
+        <v>0</v>
+      </c>
+      <c r="AH82">
+        <v>0</v>
+      </c>
+      <c r="AI82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:35">
+      <c r="A83" t="s">
+        <v>92</v>
+      </c>
+      <c r="B83" t="s">
+        <v>124</v>
+      </c>
+      <c r="C83">
+        <v>33.8547</v>
+      </c>
+      <c r="D83">
+        <v>35.8623</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+      <c r="K83">
+        <v>0</v>
+      </c>
+      <c r="L83">
+        <v>0</v>
+      </c>
+      <c r="M83">
+        <v>0</v>
+      </c>
+      <c r="N83">
+        <v>0</v>
+      </c>
+      <c r="O83">
+        <v>0</v>
+      </c>
+      <c r="P83">
+        <v>0</v>
+      </c>
+      <c r="Q83">
+        <v>0</v>
+      </c>
+      <c r="R83">
+        <v>0</v>
+      </c>
+      <c r="S83">
+        <v>0</v>
+      </c>
+      <c r="T83">
+        <v>0</v>
+      </c>
+      <c r="U83">
+        <v>0</v>
+      </c>
+      <c r="V83">
+        <v>0</v>
+      </c>
+      <c r="W83">
+        <v>0</v>
+      </c>
+      <c r="X83">
+        <v>0</v>
+      </c>
+      <c r="Y83">
+        <v>0</v>
+      </c>
+      <c r="Z83">
+        <v>0</v>
+      </c>
+      <c r="AA83">
+        <v>0</v>
+      </c>
+      <c r="AB83">
+        <v>0</v>
+      </c>
+      <c r="AC83">
+        <v>0</v>
+      </c>
+      <c r="AD83">
+        <v>0</v>
+      </c>
+      <c r="AE83">
+        <v>0</v>
+      </c>
+      <c r="AF83">
+        <v>0</v>
+      </c>
+      <c r="AG83">
+        <v>0</v>
+      </c>
+      <c r="AH83">
+        <v>0</v>
+      </c>
+      <c r="AI83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:35">
+      <c r="A84" t="s">
+        <v>93</v>
+      </c>
+      <c r="B84" t="s">
+        <v>99</v>
+      </c>
+      <c r="C84">
+        <v>40.745</v>
+      </c>
+      <c r="D84">
+        <v>-123.8695</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <v>0</v>
+      </c>
+      <c r="M84">
+        <v>0</v>
+      </c>
+      <c r="N84">
+        <v>0</v>
+      </c>
+      <c r="O84">
+        <v>0</v>
+      </c>
+      <c r="P84">
+        <v>0</v>
+      </c>
+      <c r="Q84">
+        <v>0</v>
+      </c>
+      <c r="R84">
+        <v>0</v>
+      </c>
+      <c r="S84">
+        <v>0</v>
+      </c>
+      <c r="T84">
+        <v>0</v>
+      </c>
+      <c r="U84">
+        <v>0</v>
+      </c>
+      <c r="V84">
+        <v>0</v>
+      </c>
+      <c r="W84">
+        <v>0</v>
+      </c>
+      <c r="X84">
+        <v>0</v>
+      </c>
+      <c r="Y84">
+        <v>0</v>
+      </c>
+      <c r="Z84">
+        <v>0</v>
+      </c>
+      <c r="AA84">
+        <v>0</v>
+      </c>
+      <c r="AB84">
+        <v>0</v>
+      </c>
+      <c r="AC84">
+        <v>0</v>
+      </c>
+      <c r="AD84">
+        <v>0</v>
+      </c>
+      <c r="AE84">
+        <v>0</v>
+      </c>
+      <c r="AF84">
+        <v>0</v>
+      </c>
+      <c r="AG84">
+        <v>0</v>
+      </c>
+      <c r="AH84">
+        <v>0</v>
+      </c>
+      <c r="AI84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:35">
+      <c r="A85" t="s">
+        <v>94</v>
+      </c>
+      <c r="B85" t="s">
+        <v>99</v>
+      </c>
+      <c r="C85">
+        <v>38.4747</v>
+      </c>
+      <c r="D85">
+        <v>-121.3542</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+      <c r="M85">
+        <v>0</v>
+      </c>
+      <c r="N85">
+        <v>0</v>
+      </c>
+      <c r="O85">
+        <v>0</v>
+      </c>
+      <c r="P85">
+        <v>0</v>
+      </c>
+      <c r="Q85">
+        <v>0</v>
+      </c>
+      <c r="R85">
+        <v>0</v>
+      </c>
+      <c r="S85">
+        <v>0</v>
+      </c>
+      <c r="T85">
+        <v>0</v>
+      </c>
+      <c r="U85">
+        <v>0</v>
+      </c>
+      <c r="V85">
+        <v>0</v>
+      </c>
+      <c r="W85">
+        <v>0</v>
+      </c>
+      <c r="X85">
+        <v>0</v>
+      </c>
+      <c r="Y85">
+        <v>0</v>
+      </c>
+      <c r="Z85">
+        <v>0</v>
+      </c>
+      <c r="AA85">
+        <v>0</v>
+      </c>
+      <c r="AB85">
+        <v>0</v>
+      </c>
+      <c r="AC85">
+        <v>0</v>
+      </c>
+      <c r="AD85">
+        <v>0</v>
+      </c>
+      <c r="AE85">
+        <v>0</v>
+      </c>
+      <c r="AF85">
+        <v>0</v>
+      </c>
+      <c r="AG85">
+        <v>0</v>
+      </c>
+      <c r="AH85">
+        <v>0</v>
+      </c>
+      <c r="AI85">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
check and update limit and charts
</commit_message>
<xml_diff>
--- a/COVID19-Confirmed.xlsx
+++ b/COVID19-Confirmed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="146">
   <si>
     <t>Province/State</t>
   </si>
@@ -130,6 +130,12 @@
     <t>2/24/20</t>
   </si>
   <si>
+    <t>2/25/20</t>
+  </si>
+  <si>
+    <t>2/26/20</t>
+  </si>
+  <si>
     <t>Anhui</t>
   </si>
   <si>
@@ -394,25 +400,58 @@
     <t>Iran</t>
   </si>
   <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
     <t>Israel</t>
   </si>
   <si>
-    <t>Lebanon</t>
-  </si>
-  <si>
-    <t>Iraq</t>
-  </si>
-  <si>
-    <t>Oman</t>
-  </si>
-  <si>
-    <t>Afghanistan</t>
-  </si>
-  <si>
-    <t>Bahrain</t>
-  </si>
-  <si>
-    <t>Kuwait</t>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>North Macedonia</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Romania</t>
   </si>
 </sst>
 </file>
@@ -770,13 +809,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AL91"/>
+  <dimension ref="A1:AN102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:40">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -891,13 +930,19 @@
       <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:40">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C2">
         <v>31.82571</v>
@@ -1007,13 +1052,19 @@
       <c r="AL2">
         <v>989</v>
       </c>
+      <c r="AM2">
+        <v>989</v>
+      </c>
+      <c r="AN2">
+        <v>989</v>
+      </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:40">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C3">
         <v>40.18238</v>
@@ -1123,13 +1174,19 @@
       <c r="AL3">
         <v>399</v>
       </c>
+      <c r="AM3">
+        <v>400</v>
+      </c>
+      <c r="AN3">
+        <v>400</v>
+      </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:40">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C4">
         <v>30.05718</v>
@@ -1239,13 +1296,19 @@
       <c r="AL4">
         <v>576</v>
       </c>
+      <c r="AM4">
+        <v>576</v>
+      </c>
+      <c r="AN4">
+        <v>576</v>
+      </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:40">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C5">
         <v>26.07783</v>
@@ -1355,13 +1418,19 @@
       <c r="AL5">
         <v>293</v>
       </c>
+      <c r="AM5">
+        <v>294</v>
+      </c>
+      <c r="AN5">
+        <v>294</v>
+      </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:40">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <v>36.0611</v>
@@ -1471,13 +1540,19 @@
       <c r="AL6">
         <v>91</v>
       </c>
+      <c r="AM6">
+        <v>91</v>
+      </c>
+      <c r="AN6">
+        <v>91</v>
+      </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:40">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C7">
         <v>23.33841</v>
@@ -1587,13 +1662,19 @@
       <c r="AL7">
         <v>1345</v>
       </c>
+      <c r="AM7">
+        <v>1347</v>
+      </c>
+      <c r="AN7">
+        <v>1347</v>
+      </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:40">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C8">
         <v>23.82908</v>
@@ -1703,13 +1784,19 @@
       <c r="AL8">
         <v>251</v>
       </c>
+      <c r="AM8">
+        <v>252</v>
+      </c>
+      <c r="AN8">
+        <v>252</v>
+      </c>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:40">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C9">
         <v>26.81536</v>
@@ -1819,13 +1906,19 @@
       <c r="AL9">
         <v>146</v>
       </c>
+      <c r="AM9">
+        <v>146</v>
+      </c>
+      <c r="AN9">
+        <v>146</v>
+      </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:40">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C10">
         <v>19.19673</v>
@@ -1935,13 +2028,19 @@
       <c r="AL10">
         <v>168</v>
       </c>
+      <c r="AM10">
+        <v>168</v>
+      </c>
+      <c r="AN10">
+        <v>168</v>
+      </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:40">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C11">
         <v>38.0428</v>
@@ -2051,13 +2150,19 @@
       <c r="AL11">
         <v>311</v>
       </c>
+      <c r="AM11">
+        <v>311</v>
+      </c>
+      <c r="AN11">
+        <v>312</v>
+      </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:40">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C12">
         <v>47.86199999999999</v>
@@ -2167,13 +2272,19 @@
       <c r="AL12">
         <v>480</v>
       </c>
+      <c r="AM12">
+        <v>480</v>
+      </c>
+      <c r="AN12">
+        <v>480</v>
+      </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:40">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C13">
         <v>33.88202</v>
@@ -2283,13 +2394,19 @@
       <c r="AL13">
         <v>1271</v>
       </c>
+      <c r="AM13">
+        <v>1271</v>
+      </c>
+      <c r="AN13">
+        <v>1271</v>
+      </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:40">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C14">
         <v>30.97564</v>
@@ -2399,13 +2516,19 @@
       <c r="AL14">
         <v>64287</v>
       </c>
+      <c r="AM14">
+        <v>64786</v>
+      </c>
+      <c r="AN14">
+        <v>65187</v>
+      </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:40">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C15">
         <v>27.61041</v>
@@ -2515,13 +2638,19 @@
       <c r="AL15">
         <v>1016</v>
       </c>
+      <c r="AM15">
+        <v>1016</v>
+      </c>
+      <c r="AN15">
+        <v>1016</v>
+      </c>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:40">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C16">
         <v>44.09448</v>
@@ -2631,13 +2760,19 @@
       <c r="AL16">
         <v>75</v>
       </c>
+      <c r="AM16">
+        <v>75</v>
+      </c>
+      <c r="AN16">
+        <v>75</v>
+      </c>
     </row>
-    <row r="17" spans="1:38">
+    <row r="17" spans="1:40">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C17">
         <v>32.97027</v>
@@ -2747,13 +2882,19 @@
       <c r="AL17">
         <v>631</v>
       </c>
+      <c r="AM17">
+        <v>631</v>
+      </c>
+      <c r="AN17">
+        <v>631</v>
+      </c>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:40">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C18">
         <v>27.61401</v>
@@ -2863,13 +3004,19 @@
       <c r="AL18">
         <v>934</v>
       </c>
+      <c r="AM18">
+        <v>934</v>
+      </c>
+      <c r="AN18">
+        <v>934</v>
+      </c>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:40">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C19">
         <v>43.66657</v>
@@ -2979,13 +3126,19 @@
       <c r="AL19">
         <v>93</v>
       </c>
+      <c r="AM19">
+        <v>93</v>
+      </c>
+      <c r="AN19">
+        <v>93</v>
+      </c>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:40">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C20">
         <v>41.29284000000001</v>
@@ -3095,13 +3248,19 @@
       <c r="AL20">
         <v>121</v>
       </c>
+      <c r="AM20">
+        <v>121</v>
+      </c>
+      <c r="AN20">
+        <v>121</v>
+      </c>
     </row>
-    <row r="21" spans="1:38">
+    <row r="21" spans="1:40">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C21">
         <v>37.26923</v>
@@ -3211,13 +3370,19 @@
       <c r="AL21">
         <v>71</v>
       </c>
+      <c r="AM21">
+        <v>71</v>
+      </c>
+      <c r="AN21">
+        <v>71</v>
+      </c>
     </row>
-    <row r="22" spans="1:38">
+    <row r="22" spans="1:40">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C22">
         <v>35.65945</v>
@@ -3327,13 +3492,19 @@
       <c r="AL22">
         <v>18</v>
       </c>
+      <c r="AM22">
+        <v>18</v>
+      </c>
+      <c r="AN22">
+        <v>18</v>
+      </c>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:40">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C23">
         <v>35.19165</v>
@@ -3443,13 +3614,19 @@
       <c r="AL23">
         <v>245</v>
       </c>
+      <c r="AM23">
+        <v>245</v>
+      </c>
+      <c r="AN23">
+        <v>245</v>
+      </c>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:40">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C24">
         <v>36.34377</v>
@@ -3559,13 +3736,19 @@
       <c r="AL24">
         <v>755</v>
       </c>
+      <c r="AM24">
+        <v>756</v>
+      </c>
+      <c r="AN24">
+        <v>756</v>
+      </c>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:40">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C25">
         <v>31.20327</v>
@@ -3675,13 +3858,19 @@
       <c r="AL25">
         <v>335</v>
       </c>
+      <c r="AM25">
+        <v>336</v>
+      </c>
+      <c r="AN25">
+        <v>337</v>
+      </c>
     </row>
-    <row r="26" spans="1:38">
+    <row r="26" spans="1:40">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C26">
         <v>37.57769</v>
@@ -3791,13 +3980,19 @@
       <c r="AL26">
         <v>133</v>
       </c>
+      <c r="AM26">
+        <v>133</v>
+      </c>
+      <c r="AN26">
+        <v>133</v>
+      </c>
     </row>
-    <row r="27" spans="1:38">
+    <row r="27" spans="1:40">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C27">
         <v>30.61714</v>
@@ -3907,13 +4102,19 @@
       <c r="AL27">
         <v>527</v>
       </c>
+      <c r="AM27">
+        <v>529</v>
+      </c>
+      <c r="AN27">
+        <v>531</v>
+      </c>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:40">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C28">
         <v>39.29362</v>
@@ -4023,13 +4224,19 @@
       <c r="AL28">
         <v>135</v>
       </c>
+      <c r="AM28">
+        <v>135</v>
+      </c>
+      <c r="AN28">
+        <v>135</v>
+      </c>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:40">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C29">
         <v>30.1534</v>
@@ -4139,13 +4346,19 @@
       <c r="AL29">
         <v>1</v>
       </c>
+      <c r="AM29">
+        <v>1</v>
+      </c>
+      <c r="AN29">
+        <v>1</v>
+      </c>
     </row>
-    <row r="30" spans="1:38">
+    <row r="30" spans="1:40">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C30">
         <v>41.11981</v>
@@ -4255,13 +4468,19 @@
       <c r="AL30">
         <v>76</v>
       </c>
+      <c r="AM30">
+        <v>76</v>
+      </c>
+      <c r="AN30">
+        <v>76</v>
+      </c>
     </row>
-    <row r="31" spans="1:38">
+    <row r="31" spans="1:40">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B31" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C31">
         <v>24.97411</v>
@@ -4371,13 +4590,19 @@
       <c r="AL31">
         <v>174</v>
       </c>
+      <c r="AM31">
+        <v>174</v>
+      </c>
+      <c r="AN31">
+        <v>174</v>
+      </c>
     </row>
-    <row r="32" spans="1:38">
+    <row r="32" spans="1:40">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C32">
         <v>29.18251</v>
@@ -4487,10 +4712,16 @@
       <c r="AL32">
         <v>1205</v>
       </c>
+      <c r="AM32">
+        <v>1205</v>
+      </c>
+      <c r="AN32">
+        <v>1205</v>
+      </c>
     </row>
-    <row r="33" spans="1:38">
+    <row r="33" spans="1:40">
       <c r="B33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C33">
         <v>13.7563</v>
@@ -4600,10 +4831,16 @@
       <c r="AL33">
         <v>35</v>
       </c>
+      <c r="AM33">
+        <v>37</v>
+      </c>
+      <c r="AN33">
+        <v>40</v>
+      </c>
     </row>
-    <row r="34" spans="1:38">
+    <row r="34" spans="1:40">
       <c r="B34" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C34">
         <v>35.6762</v>
@@ -4713,10 +4950,16 @@
       <c r="AL34">
         <v>159</v>
       </c>
+      <c r="AM34">
+        <v>170</v>
+      </c>
+      <c r="AN34">
+        <v>189</v>
+      </c>
     </row>
-    <row r="35" spans="1:38">
+    <row r="35" spans="1:40">
       <c r="B35" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C35">
         <v>37.5665</v>
@@ -4826,13 +5069,19 @@
       <c r="AL35">
         <v>833</v>
       </c>
+      <c r="AM35">
+        <v>977</v>
+      </c>
+      <c r="AN35">
+        <v>1261</v>
+      </c>
     </row>
-    <row r="36" spans="1:38">
+    <row r="36" spans="1:40">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C36">
         <v>23.6978</v>
@@ -4942,13 +5191,19 @@
       <c r="AL36">
         <v>30</v>
       </c>
+      <c r="AM36">
+        <v>31</v>
+      </c>
+      <c r="AN36">
+        <v>32</v>
+      </c>
     </row>
-    <row r="37" spans="1:38">
+    <row r="37" spans="1:40">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C37">
         <v>47.7511</v>
@@ -5058,13 +5313,19 @@
       <c r="AL37">
         <v>1</v>
       </c>
+      <c r="AM37">
+        <v>1</v>
+      </c>
+      <c r="AN37">
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="1:38">
+    <row r="38" spans="1:40">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C38">
         <v>40.6331</v>
@@ -5174,13 +5435,19 @@
       <c r="AL38">
         <v>2</v>
       </c>
+      <c r="AM38">
+        <v>2</v>
+      </c>
+      <c r="AN38">
+        <v>2</v>
+      </c>
     </row>
-    <row r="39" spans="1:38">
+    <row r="39" spans="1:40">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C39">
         <v>34.0489</v>
@@ -5290,13 +5557,19 @@
       <c r="AL39">
         <v>1</v>
       </c>
+      <c r="AM39">
+        <v>1</v>
+      </c>
+      <c r="AN39">
+        <v>1</v>
+      </c>
     </row>
-    <row r="40" spans="1:38">
+    <row r="40" spans="1:40">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B40" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C40">
         <v>22.1987</v>
@@ -5406,13 +5679,19 @@
       <c r="AL40">
         <v>10</v>
       </c>
+      <c r="AM40">
+        <v>10</v>
+      </c>
+      <c r="AN40">
+        <v>10</v>
+      </c>
     </row>
-    <row r="41" spans="1:38">
+    <row r="41" spans="1:40">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B41" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C41">
         <v>22.3193</v>
@@ -5522,10 +5801,16 @@
       <c r="AL41">
         <v>79</v>
       </c>
+      <c r="AM41">
+        <v>84</v>
+      </c>
+      <c r="AN41">
+        <v>91</v>
+      </c>
     </row>
-    <row r="42" spans="1:38">
+    <row r="42" spans="1:40">
       <c r="B42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C42">
         <v>1.3521</v>
@@ -5635,10 +5920,16 @@
       <c r="AL42">
         <v>89</v>
       </c>
+      <c r="AM42">
+        <v>91</v>
+      </c>
+      <c r="AN42">
+        <v>93</v>
+      </c>
     </row>
-    <row r="43" spans="1:38">
+    <row r="43" spans="1:40">
       <c r="B43" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C43">
         <v>21.0278</v>
@@ -5748,10 +6039,16 @@
       <c r="AL43">
         <v>16</v>
       </c>
+      <c r="AM43">
+        <v>16</v>
+      </c>
+      <c r="AN43">
+        <v>16</v>
+      </c>
     </row>
-    <row r="44" spans="1:38">
+    <row r="44" spans="1:40">
       <c r="B44" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C44">
         <v>46.2276</v>
@@ -5861,10 +6158,16 @@
       <c r="AL44">
         <v>12</v>
       </c>
+      <c r="AM44">
+        <v>14</v>
+      </c>
+      <c r="AN44">
+        <v>18</v>
+      </c>
     </row>
-    <row r="45" spans="1:38">
+    <row r="45" spans="1:40">
       <c r="B45" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C45">
         <v>28.3949</v>
@@ -5974,10 +6277,16 @@
       <c r="AL45">
         <v>1</v>
       </c>
+      <c r="AM45">
+        <v>1</v>
+      </c>
+      <c r="AN45">
+        <v>1</v>
+      </c>
     </row>
-    <row r="46" spans="1:38">
+    <row r="46" spans="1:40">
       <c r="B46" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C46">
         <v>4.2105</v>
@@ -6087,13 +6396,19 @@
       <c r="AL46">
         <v>22</v>
       </c>
+      <c r="AM46">
+        <v>22</v>
+      </c>
+      <c r="AN46">
+        <v>22</v>
+      </c>
     </row>
-    <row r="47" spans="1:38">
+    <row r="47" spans="1:40">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B47" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C47">
         <v>43.6532</v>
@@ -6203,13 +6518,19 @@
       <c r="AL47">
         <v>3</v>
       </c>
+      <c r="AM47">
+        <v>3</v>
+      </c>
+      <c r="AN47">
+        <v>3</v>
+      </c>
     </row>
-    <row r="48" spans="1:38">
+    <row r="48" spans="1:40">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C48">
         <v>49.2827</v>
@@ -6319,13 +6640,19 @@
       <c r="AL48">
         <v>6</v>
       </c>
+      <c r="AM48">
+        <v>7</v>
+      </c>
+      <c r="AN48">
+        <v>7</v>
+      </c>
     </row>
-    <row r="49" spans="1:38">
+    <row r="49" spans="1:40">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C49">
         <v>33.7879</v>
@@ -6435,13 +6762,19 @@
       <c r="AL49">
         <v>1</v>
       </c>
+      <c r="AM49">
+        <v>1</v>
+      </c>
+      <c r="AN49">
+        <v>1</v>
+      </c>
     </row>
-    <row r="50" spans="1:38">
+    <row r="50" spans="1:40">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C50">
         <v>34.0522</v>
@@ -6551,13 +6884,19 @@
       <c r="AL50">
         <v>1</v>
       </c>
+      <c r="AM50">
+        <v>1</v>
+      </c>
+      <c r="AN50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="1:38">
+    <row r="51" spans="1:40">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B51" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C51">
         <v>-33.8688</v>
@@ -6667,13 +7006,19 @@
       <c r="AL51">
         <v>4</v>
       </c>
+      <c r="AM51">
+        <v>4</v>
+      </c>
+      <c r="AN51">
+        <v>4</v>
+      </c>
     </row>
-    <row r="52" spans="1:38">
+    <row r="52" spans="1:40">
       <c r="A52" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B52" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C52">
         <v>-37.8136</v>
@@ -6783,13 +7128,19 @@
       <c r="AL52">
         <v>4</v>
       </c>
+      <c r="AM52">
+        <v>4</v>
+      </c>
+      <c r="AN52">
+        <v>4</v>
+      </c>
     </row>
-    <row r="53" spans="1:38">
+    <row r="53" spans="1:40">
       <c r="A53" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B53" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C53">
         <v>-27.4698</v>
@@ -6899,10 +7250,16 @@
       <c r="AL53">
         <v>5</v>
       </c>
+      <c r="AM53">
+        <v>5</v>
+      </c>
+      <c r="AN53">
+        <v>5</v>
+      </c>
     </row>
-    <row r="54" spans="1:38">
+    <row r="54" spans="1:40">
       <c r="B54" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C54">
         <v>12.5657</v>
@@ -7012,10 +7369,16 @@
       <c r="AL54">
         <v>1</v>
       </c>
+      <c r="AM54">
+        <v>1</v>
+      </c>
+      <c r="AN54">
+        <v>1</v>
+      </c>
     </row>
-    <row r="55" spans="1:38">
+    <row r="55" spans="1:40">
       <c r="B55" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C55">
         <v>7.8731</v>
@@ -7125,10 +7488,16 @@
       <c r="AL55">
         <v>1</v>
       </c>
+      <c r="AM55">
+        <v>1</v>
+      </c>
+      <c r="AN55">
+        <v>1</v>
+      </c>
     </row>
-    <row r="56" spans="1:38">
+    <row r="56" spans="1:40">
       <c r="B56" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C56">
         <v>51.1657</v>
@@ -7238,10 +7607,16 @@
       <c r="AL56">
         <v>16</v>
       </c>
+      <c r="AM56">
+        <v>17</v>
+      </c>
+      <c r="AN56">
+        <v>27</v>
+      </c>
     </row>
-    <row r="57" spans="1:38">
+    <row r="57" spans="1:40">
       <c r="B57" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C57">
         <v>61.9241</v>
@@ -7351,10 +7726,16 @@
       <c r="AL57">
         <v>1</v>
       </c>
+      <c r="AM57">
+        <v>1</v>
+      </c>
+      <c r="AN57">
+        <v>2</v>
+      </c>
     </row>
-    <row r="58" spans="1:38">
+    <row r="58" spans="1:40">
       <c r="B58" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C58">
         <v>23.4241</v>
@@ -7464,10 +7845,16 @@
       <c r="AL58">
         <v>13</v>
       </c>
+      <c r="AM58">
+        <v>13</v>
+      </c>
+      <c r="AN58">
+        <v>13</v>
+      </c>
     </row>
-    <row r="59" spans="1:38">
+    <row r="59" spans="1:40">
       <c r="B59" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C59">
         <v>12.8797</v>
@@ -7577,10 +7964,16 @@
       <c r="AL59">
         <v>3</v>
       </c>
+      <c r="AM59">
+        <v>3</v>
+      </c>
+      <c r="AN59">
+        <v>3</v>
+      </c>
     </row>
-    <row r="60" spans="1:38">
+    <row r="60" spans="1:40">
       <c r="B60" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C60">
         <v>20.5937</v>
@@ -7690,13 +8083,19 @@
       <c r="AL60">
         <v>3</v>
       </c>
+      <c r="AM60">
+        <v>3</v>
+      </c>
+      <c r="AN60">
+        <v>3</v>
+      </c>
     </row>
-    <row r="61" spans="1:38">
+    <row r="61" spans="1:40">
       <c r="A61" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B61" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C61">
         <v>42.9849</v>
@@ -7806,10 +8205,16 @@
       <c r="AL61">
         <v>1</v>
       </c>
+      <c r="AM61">
+        <v>1</v>
+      </c>
+      <c r="AN61">
+        <v>1</v>
+      </c>
     </row>
-    <row r="62" spans="1:38">
+    <row r="62" spans="1:40">
       <c r="B62" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C62">
         <v>41.8719</v>
@@ -7919,10 +8324,16 @@
       <c r="AL62">
         <v>229</v>
       </c>
+      <c r="AM62">
+        <v>322</v>
+      </c>
+      <c r="AN62">
+        <v>453</v>
+      </c>
     </row>
-    <row r="63" spans="1:38">
+    <row r="63" spans="1:40">
       <c r="B63" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C63">
         <v>55.3781</v>
@@ -8032,10 +8443,16 @@
       <c r="AL63">
         <v>13</v>
       </c>
+      <c r="AM63">
+        <v>13</v>
+      </c>
+      <c r="AN63">
+        <v>13</v>
+      </c>
     </row>
-    <row r="64" spans="1:38">
+    <row r="64" spans="1:40">
       <c r="B64" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C64">
         <v>61.52399999999999</v>
@@ -8145,10 +8562,16 @@
       <c r="AL64">
         <v>2</v>
       </c>
+      <c r="AM64">
+        <v>2</v>
+      </c>
+      <c r="AN64">
+        <v>2</v>
+      </c>
     </row>
-    <row r="65" spans="1:38">
+    <row r="65" spans="1:40">
       <c r="B65" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C65">
         <v>60.1282</v>
@@ -8258,13 +8681,19 @@
       <c r="AL65">
         <v>1</v>
       </c>
+      <c r="AM65">
+        <v>1</v>
+      </c>
+      <c r="AN65">
+        <v>2</v>
+      </c>
     </row>
-    <row r="66" spans="1:38">
+    <row r="66" spans="1:40">
       <c r="A66" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B66" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C66">
         <v>37.3541</v>
@@ -8374,10 +8803,16 @@
       <c r="AL66">
         <v>2</v>
       </c>
+      <c r="AM66">
+        <v>2</v>
+      </c>
+      <c r="AN66">
+        <v>2</v>
+      </c>
     </row>
-    <row r="67" spans="1:38">
+    <row r="67" spans="1:40">
       <c r="B67" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C67">
         <v>40.4637</v>
@@ -8487,13 +8922,19 @@
       <c r="AL67">
         <v>2</v>
       </c>
+      <c r="AM67">
+        <v>6</v>
+      </c>
+      <c r="AN67">
+        <v>13</v>
+      </c>
     </row>
-    <row r="68" spans="1:38">
+    <row r="68" spans="1:40">
       <c r="A68" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B68" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C68">
         <v>-34.9285</v>
@@ -8603,13 +9044,19 @@
       <c r="AL68">
         <v>2</v>
       </c>
+      <c r="AM68">
+        <v>2</v>
+      </c>
+      <c r="AN68">
+        <v>2</v>
+      </c>
     </row>
-    <row r="69" spans="1:38">
+    <row r="69" spans="1:40">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B69" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C69">
         <v>42.3601</v>
@@ -8719,13 +9166,19 @@
       <c r="AL69">
         <v>1</v>
       </c>
+      <c r="AM69">
+        <v>1</v>
+      </c>
+      <c r="AN69">
+        <v>1</v>
+      </c>
     </row>
-    <row r="70" spans="1:38">
+    <row r="70" spans="1:40">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B70" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C70">
         <v>36.5761</v>
@@ -8835,10 +9288,16 @@
       <c r="AL70">
         <v>2</v>
       </c>
+      <c r="AM70">
+        <v>2</v>
+      </c>
+      <c r="AN70">
+        <v>2</v>
+      </c>
     </row>
-    <row r="71" spans="1:38">
+    <row r="71" spans="1:40">
       <c r="B71" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C71">
         <v>50.5039</v>
@@ -8948,13 +9407,19 @@
       <c r="AL71">
         <v>1</v>
       </c>
+      <c r="AM71">
+        <v>1</v>
+      </c>
+      <c r="AN71">
+        <v>1</v>
+      </c>
     </row>
-    <row r="72" spans="1:38">
+    <row r="72" spans="1:40">
       <c r="A72" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B72" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C72">
         <v>43.0731</v>
@@ -9064,13 +9529,19 @@
       <c r="AL72">
         <v>1</v>
       </c>
+      <c r="AM72">
+        <v>1</v>
+      </c>
+      <c r="AN72">
+        <v>1</v>
+      </c>
     </row>
-    <row r="73" spans="1:38">
+    <row r="73" spans="1:40">
       <c r="A73" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B73" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C73">
         <v>35.4437</v>
@@ -9180,13 +9651,19 @@
       <c r="AL73">
         <v>691</v>
       </c>
+      <c r="AM73">
+        <v>691</v>
+      </c>
+      <c r="AN73">
+        <v>705</v>
+      </c>
     </row>
-    <row r="74" spans="1:38">
+    <row r="74" spans="1:40">
       <c r="A74" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B74" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C74">
         <v>32.7157</v>
@@ -9296,13 +9773,19 @@
       <c r="AL74">
         <v>2</v>
       </c>
+      <c r="AM74">
+        <v>2</v>
+      </c>
+      <c r="AN74">
+        <v>2</v>
+      </c>
     </row>
-    <row r="75" spans="1:38">
+    <row r="75" spans="1:40">
       <c r="A75" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B75" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C75">
         <v>29.4241</v>
@@ -9412,10 +9895,16 @@
       <c r="AL75">
         <v>1</v>
       </c>
+      <c r="AM75">
+        <v>1</v>
+      </c>
+      <c r="AN75">
+        <v>1</v>
+      </c>
     </row>
-    <row r="76" spans="1:38">
+    <row r="76" spans="1:40">
       <c r="B76" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C76">
         <v>26.8206</v>
@@ -9525,10 +10014,16 @@
       <c r="AL76">
         <v>1</v>
       </c>
+      <c r="AM76">
+        <v>1</v>
+      </c>
+      <c r="AN76">
+        <v>1</v>
+      </c>
     </row>
-    <row r="77" spans="1:38">
+    <row r="77" spans="1:40">
       <c r="B77" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C77">
         <v>32.4279</v>
@@ -9638,13 +10133,19 @@
       <c r="AL77">
         <v>61</v>
       </c>
+      <c r="AM77">
+        <v>95</v>
+      </c>
+      <c r="AN77">
+        <v>139</v>
+      </c>
     </row>
-    <row r="78" spans="1:38">
+    <row r="78" spans="1:40">
       <c r="A78" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B78" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C78">
         <v>41.2545</v>
@@ -9754,13 +10255,19 @@
       <c r="AL78">
         <v>0</v>
       </c>
+      <c r="AM78">
+        <v>0</v>
+      </c>
+      <c r="AN78">
+        <v>0</v>
+      </c>
     </row>
-    <row r="79" spans="1:38">
+    <row r="79" spans="1:40">
       <c r="A79" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B79" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C79">
         <v>38.2721</v>
@@ -9870,13 +10377,19 @@
       <c r="AL79">
         <v>0</v>
       </c>
+      <c r="AM79">
+        <v>0</v>
+      </c>
+      <c r="AN79">
+        <v>0</v>
+      </c>
     </row>
-    <row r="80" spans="1:38">
+    <row r="80" spans="1:40">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B80" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C80">
         <v>35.4437</v>
@@ -9986,13 +10499,19 @@
       <c r="AL80">
         <v>7</v>
       </c>
+      <c r="AM80">
+        <v>7</v>
+      </c>
+      <c r="AN80">
+        <v>7</v>
+      </c>
     </row>
-    <row r="81" spans="1:38">
+    <row r="81" spans="1:40">
       <c r="A81" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B81" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C81">
         <v>29.3829</v>
@@ -10102,19 +10621,22 @@
       <c r="AL81">
         <v>0</v>
       </c>
+      <c r="AM81">
+        <v>0</v>
+      </c>
+      <c r="AN81">
+        <v>0</v>
+      </c>
     </row>
-    <row r="82" spans="1:38">
-      <c r="A82" t="s">
-        <v>93</v>
-      </c>
+    <row r="82" spans="1:40">
       <c r="B82" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C82">
-        <v>31.0461</v>
+        <v>33.8547</v>
       </c>
       <c r="D82">
-        <v>34.8516</v>
+        <v>35.8623</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -10218,16 +10740,25 @@
       <c r="AL82">
         <v>1</v>
       </c>
+      <c r="AM82">
+        <v>1</v>
+      </c>
+      <c r="AN82">
+        <v>2</v>
+      </c>
     </row>
-    <row r="83" spans="1:38">
+    <row r="83" spans="1:40">
+      <c r="A83" t="s">
+        <v>97</v>
+      </c>
       <c r="B83" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="C83">
-        <v>33.8547</v>
+        <v>40.745</v>
       </c>
       <c r="D83">
-        <v>35.8623</v>
+        <v>-123.8695</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -10331,19 +10862,25 @@
       <c r="AL83">
         <v>1</v>
       </c>
+      <c r="AM83">
+        <v>1</v>
+      </c>
+      <c r="AN83">
+        <v>1</v>
+      </c>
     </row>
-    <row r="84" spans="1:38">
+    <row r="84" spans="1:40">
       <c r="A84" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B84" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C84">
-        <v>40.745</v>
+        <v>38.4747</v>
       </c>
       <c r="D84">
-        <v>-123.8695</v>
+        <v>-121.3542</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -10447,19 +10984,22 @@
       <c r="AL84">
         <v>1</v>
       </c>
+      <c r="AM84">
+        <v>1</v>
+      </c>
+      <c r="AN84">
+        <v>1</v>
+      </c>
     </row>
-    <row r="85" spans="1:38">
-      <c r="A85" t="s">
-        <v>96</v>
-      </c>
+    <row r="85" spans="1:40">
       <c r="B85" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="C85">
-        <v>38.4747</v>
+        <v>33.2232</v>
       </c>
       <c r="D85">
-        <v>-121.3542</v>
+        <v>43.6793</v>
       </c>
       <c r="E85">
         <v>0</v>
@@ -10552,27 +11092,36 @@
         <v>0</v>
       </c>
       <c r="AI85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL85">
         <v>1</v>
       </c>
+      <c r="AM85">
+        <v>1</v>
+      </c>
+      <c r="AN85">
+        <v>5</v>
+      </c>
     </row>
-    <row r="86" spans="1:38">
+    <row r="86" spans="1:40">
+      <c r="A86" t="s">
+        <v>99</v>
+      </c>
       <c r="B86" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="C86">
-        <v>33.2232</v>
+        <v>37.0902</v>
       </c>
       <c r="D86">
-        <v>43.6793</v>
+        <v>-95.7129</v>
       </c>
       <c r="E86">
         <v>0</v>
@@ -10674,21 +11223,24 @@
         <v>0</v>
       </c>
       <c r="AL86">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="AM86">
+        <v>36</v>
+      </c>
+      <c r="AN86">
+        <v>42</v>
       </c>
     </row>
-    <row r="87" spans="1:38">
-      <c r="A87" t="s">
-        <v>97</v>
-      </c>
+    <row r="87" spans="1:40">
       <c r="B87" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="C87">
-        <v>37.0902</v>
+        <v>21.4735</v>
       </c>
       <c r="D87">
-        <v>-95.7129</v>
+        <v>55.9754</v>
       </c>
       <c r="E87">
         <v>0</v>
@@ -10790,18 +11342,24 @@
         <v>0</v>
       </c>
       <c r="AL87">
-        <v>36</v>
+        <v>2</v>
+      </c>
+      <c r="AM87">
+        <v>2</v>
+      </c>
+      <c r="AN87">
+        <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:38">
+    <row r="88" spans="1:40">
       <c r="B88" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C88">
-        <v>21.4735</v>
+        <v>33</v>
       </c>
       <c r="D88">
-        <v>55.9754</v>
+        <v>65</v>
       </c>
       <c r="E88">
         <v>0</v>
@@ -10903,131 +11461,143 @@
         <v>0</v>
       </c>
       <c r="AL88">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="AM88">
+        <v>1</v>
+      </c>
+      <c r="AN88">
+        <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:38">
+    <row r="89" spans="1:40">
       <c r="B89" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C89">
+        <v>26.0275</v>
+      </c>
+      <c r="D89">
+        <v>50.55</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+      <c r="K89">
+        <v>0</v>
+      </c>
+      <c r="L89">
+        <v>0</v>
+      </c>
+      <c r="M89">
+        <v>0</v>
+      </c>
+      <c r="N89">
+        <v>0</v>
+      </c>
+      <c r="O89">
+        <v>0</v>
+      </c>
+      <c r="P89">
+        <v>0</v>
+      </c>
+      <c r="Q89">
+        <v>0</v>
+      </c>
+      <c r="R89">
+        <v>0</v>
+      </c>
+      <c r="S89">
+        <v>0</v>
+      </c>
+      <c r="T89">
+        <v>0</v>
+      </c>
+      <c r="U89">
+        <v>0</v>
+      </c>
+      <c r="V89">
+        <v>0</v>
+      </c>
+      <c r="W89">
+        <v>0</v>
+      </c>
+      <c r="X89">
+        <v>0</v>
+      </c>
+      <c r="Y89">
+        <v>0</v>
+      </c>
+      <c r="Z89">
+        <v>0</v>
+      </c>
+      <c r="AA89">
+        <v>0</v>
+      </c>
+      <c r="AB89">
+        <v>0</v>
+      </c>
+      <c r="AC89">
+        <v>0</v>
+      </c>
+      <c r="AD89">
+        <v>0</v>
+      </c>
+      <c r="AE89">
+        <v>0</v>
+      </c>
+      <c r="AF89">
+        <v>0</v>
+      </c>
+      <c r="AG89">
+        <v>0</v>
+      </c>
+      <c r="AH89">
+        <v>0</v>
+      </c>
+      <c r="AI89">
+        <v>0</v>
+      </c>
+      <c r="AJ89">
+        <v>0</v>
+      </c>
+      <c r="AK89">
+        <v>0</v>
+      </c>
+      <c r="AL89">
+        <v>1</v>
+      </c>
+      <c r="AM89">
+        <v>23</v>
+      </c>
+      <c r="AN89">
         <v>33</v>
       </c>
-      <c r="D89">
-        <v>65</v>
-      </c>
-      <c r="E89">
-        <v>0</v>
-      </c>
-      <c r="F89">
-        <v>0</v>
-      </c>
-      <c r="G89">
-        <v>0</v>
-      </c>
-      <c r="H89">
-        <v>0</v>
-      </c>
-      <c r="I89">
-        <v>0</v>
-      </c>
-      <c r="J89">
-        <v>0</v>
-      </c>
-      <c r="K89">
-        <v>0</v>
-      </c>
-      <c r="L89">
-        <v>0</v>
-      </c>
-      <c r="M89">
-        <v>0</v>
-      </c>
-      <c r="N89">
-        <v>0</v>
-      </c>
-      <c r="O89">
-        <v>0</v>
-      </c>
-      <c r="P89">
-        <v>0</v>
-      </c>
-      <c r="Q89">
-        <v>0</v>
-      </c>
-      <c r="R89">
-        <v>0</v>
-      </c>
-      <c r="S89">
-        <v>0</v>
-      </c>
-      <c r="T89">
-        <v>0</v>
-      </c>
-      <c r="U89">
-        <v>0</v>
-      </c>
-      <c r="V89">
-        <v>0</v>
-      </c>
-      <c r="W89">
-        <v>0</v>
-      </c>
-      <c r="X89">
-        <v>0</v>
-      </c>
-      <c r="Y89">
-        <v>0</v>
-      </c>
-      <c r="Z89">
-        <v>0</v>
-      </c>
-      <c r="AA89">
-        <v>0</v>
-      </c>
-      <c r="AB89">
-        <v>0</v>
-      </c>
-      <c r="AC89">
-        <v>0</v>
-      </c>
-      <c r="AD89">
-        <v>0</v>
-      </c>
-      <c r="AE89">
-        <v>0</v>
-      </c>
-      <c r="AF89">
-        <v>0</v>
-      </c>
-      <c r="AG89">
-        <v>0</v>
-      </c>
-      <c r="AH89">
-        <v>0</v>
-      </c>
-      <c r="AI89">
-        <v>0</v>
-      </c>
-      <c r="AJ89">
-        <v>0</v>
-      </c>
-      <c r="AK89">
-        <v>0</v>
-      </c>
-      <c r="AL89">
-        <v>1</v>
-      </c>
     </row>
-    <row r="90" spans="1:38">
+    <row r="90" spans="1:40">
       <c r="B90" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C90">
-        <v>26.0275</v>
+        <v>29.5</v>
       </c>
       <c r="D90">
-        <v>50.55</v>
+        <v>47.75</v>
       </c>
       <c r="E90">
         <v>0</v>
@@ -11131,16 +11701,22 @@
       <c r="AL90">
         <v>1</v>
       </c>
+      <c r="AM90">
+        <v>11</v>
+      </c>
+      <c r="AN90">
+        <v>26</v>
+      </c>
     </row>
-    <row r="91" spans="1:38">
+    <row r="91" spans="1:40">
       <c r="B91" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C91">
-        <v>29.5</v>
+        <v>28.0339</v>
       </c>
       <c r="D91">
-        <v>47.75</v>
+        <v>1.6596</v>
       </c>
       <c r="E91">
         <v>0</v>
@@ -11242,6 +11818,1321 @@
         <v>0</v>
       </c>
       <c r="AL91">
+        <v>0</v>
+      </c>
+      <c r="AM91">
+        <v>1</v>
+      </c>
+      <c r="AN91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:40">
+      <c r="B92" t="s">
+        <v>135</v>
+      </c>
+      <c r="C92">
+        <v>45.1</v>
+      </c>
+      <c r="D92">
+        <v>15.2</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92">
+        <v>0</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+      <c r="K92">
+        <v>0</v>
+      </c>
+      <c r="L92">
+        <v>0</v>
+      </c>
+      <c r="M92">
+        <v>0</v>
+      </c>
+      <c r="N92">
+        <v>0</v>
+      </c>
+      <c r="O92">
+        <v>0</v>
+      </c>
+      <c r="P92">
+        <v>0</v>
+      </c>
+      <c r="Q92">
+        <v>0</v>
+      </c>
+      <c r="R92">
+        <v>0</v>
+      </c>
+      <c r="S92">
+        <v>0</v>
+      </c>
+      <c r="T92">
+        <v>0</v>
+      </c>
+      <c r="U92">
+        <v>0</v>
+      </c>
+      <c r="V92">
+        <v>0</v>
+      </c>
+      <c r="W92">
+        <v>0</v>
+      </c>
+      <c r="X92">
+        <v>0</v>
+      </c>
+      <c r="Y92">
+        <v>0</v>
+      </c>
+      <c r="Z92">
+        <v>0</v>
+      </c>
+      <c r="AA92">
+        <v>0</v>
+      </c>
+      <c r="AB92">
+        <v>0</v>
+      </c>
+      <c r="AC92">
+        <v>0</v>
+      </c>
+      <c r="AD92">
+        <v>0</v>
+      </c>
+      <c r="AE92">
+        <v>0</v>
+      </c>
+      <c r="AF92">
+        <v>0</v>
+      </c>
+      <c r="AG92">
+        <v>0</v>
+      </c>
+      <c r="AH92">
+        <v>0</v>
+      </c>
+      <c r="AI92">
+        <v>0</v>
+      </c>
+      <c r="AJ92">
+        <v>0</v>
+      </c>
+      <c r="AK92">
+        <v>0</v>
+      </c>
+      <c r="AL92">
+        <v>0</v>
+      </c>
+      <c r="AM92">
+        <v>1</v>
+      </c>
+      <c r="AN92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:40">
+      <c r="B93" t="s">
+        <v>136</v>
+      </c>
+      <c r="C93">
+        <v>46.8182</v>
+      </c>
+      <c r="D93">
+        <v>8.227499999999999</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <v>0</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
+      <c r="L93">
+        <v>0</v>
+      </c>
+      <c r="M93">
+        <v>0</v>
+      </c>
+      <c r="N93">
+        <v>0</v>
+      </c>
+      <c r="O93">
+        <v>0</v>
+      </c>
+      <c r="P93">
+        <v>0</v>
+      </c>
+      <c r="Q93">
+        <v>0</v>
+      </c>
+      <c r="R93">
+        <v>0</v>
+      </c>
+      <c r="S93">
+        <v>0</v>
+      </c>
+      <c r="T93">
+        <v>0</v>
+      </c>
+      <c r="U93">
+        <v>0</v>
+      </c>
+      <c r="V93">
+        <v>0</v>
+      </c>
+      <c r="W93">
+        <v>0</v>
+      </c>
+      <c r="X93">
+        <v>0</v>
+      </c>
+      <c r="Y93">
+        <v>0</v>
+      </c>
+      <c r="Z93">
+        <v>0</v>
+      </c>
+      <c r="AA93">
+        <v>0</v>
+      </c>
+      <c r="AB93">
+        <v>0</v>
+      </c>
+      <c r="AC93">
+        <v>0</v>
+      </c>
+      <c r="AD93">
+        <v>0</v>
+      </c>
+      <c r="AE93">
+        <v>0</v>
+      </c>
+      <c r="AF93">
+        <v>0</v>
+      </c>
+      <c r="AG93">
+        <v>0</v>
+      </c>
+      <c r="AH93">
+        <v>0</v>
+      </c>
+      <c r="AI93">
+        <v>0</v>
+      </c>
+      <c r="AJ93">
+        <v>0</v>
+      </c>
+      <c r="AK93">
+        <v>0</v>
+      </c>
+      <c r="AL93">
+        <v>0</v>
+      </c>
+      <c r="AM93">
+        <v>1</v>
+      </c>
+      <c r="AN93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:40">
+      <c r="B94" t="s">
+        <v>137</v>
+      </c>
+      <c r="C94">
+        <v>47.5162</v>
+      </c>
+      <c r="D94">
+        <v>14.5501</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+      <c r="I94">
+        <v>0</v>
+      </c>
+      <c r="J94">
+        <v>0</v>
+      </c>
+      <c r="K94">
+        <v>0</v>
+      </c>
+      <c r="L94">
+        <v>0</v>
+      </c>
+      <c r="M94">
+        <v>0</v>
+      </c>
+      <c r="N94">
+        <v>0</v>
+      </c>
+      <c r="O94">
+        <v>0</v>
+      </c>
+      <c r="P94">
+        <v>0</v>
+      </c>
+      <c r="Q94">
+        <v>0</v>
+      </c>
+      <c r="R94">
+        <v>0</v>
+      </c>
+      <c r="S94">
+        <v>0</v>
+      </c>
+      <c r="T94">
+        <v>0</v>
+      </c>
+      <c r="U94">
+        <v>0</v>
+      </c>
+      <c r="V94">
+        <v>0</v>
+      </c>
+      <c r="W94">
+        <v>0</v>
+      </c>
+      <c r="X94">
+        <v>0</v>
+      </c>
+      <c r="Y94">
+        <v>0</v>
+      </c>
+      <c r="Z94">
+        <v>0</v>
+      </c>
+      <c r="AA94">
+        <v>0</v>
+      </c>
+      <c r="AB94">
+        <v>0</v>
+      </c>
+      <c r="AC94">
+        <v>0</v>
+      </c>
+      <c r="AD94">
+        <v>0</v>
+      </c>
+      <c r="AE94">
+        <v>0</v>
+      </c>
+      <c r="AF94">
+        <v>0</v>
+      </c>
+      <c r="AG94">
+        <v>0</v>
+      </c>
+      <c r="AH94">
+        <v>0</v>
+      </c>
+      <c r="AI94">
+        <v>0</v>
+      </c>
+      <c r="AJ94">
+        <v>0</v>
+      </c>
+      <c r="AK94">
+        <v>0</v>
+      </c>
+      <c r="AL94">
+        <v>0</v>
+      </c>
+      <c r="AM94">
+        <v>2</v>
+      </c>
+      <c r="AN94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:40">
+      <c r="B95" t="s">
+        <v>138</v>
+      </c>
+      <c r="C95">
+        <v>31</v>
+      </c>
+      <c r="D95">
+        <v>35</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <v>0</v>
+      </c>
+      <c r="J95">
+        <v>0</v>
+      </c>
+      <c r="K95">
+        <v>0</v>
+      </c>
+      <c r="L95">
+        <v>0</v>
+      </c>
+      <c r="M95">
+        <v>0</v>
+      </c>
+      <c r="N95">
+        <v>0</v>
+      </c>
+      <c r="O95">
+        <v>0</v>
+      </c>
+      <c r="P95">
+        <v>0</v>
+      </c>
+      <c r="Q95">
+        <v>0</v>
+      </c>
+      <c r="R95">
+        <v>0</v>
+      </c>
+      <c r="S95">
+        <v>0</v>
+      </c>
+      <c r="T95">
+        <v>0</v>
+      </c>
+      <c r="U95">
+        <v>0</v>
+      </c>
+      <c r="V95">
+        <v>0</v>
+      </c>
+      <c r="W95">
+        <v>0</v>
+      </c>
+      <c r="X95">
+        <v>0</v>
+      </c>
+      <c r="Y95">
+        <v>0</v>
+      </c>
+      <c r="Z95">
+        <v>0</v>
+      </c>
+      <c r="AA95">
+        <v>0</v>
+      </c>
+      <c r="AB95">
+        <v>0</v>
+      </c>
+      <c r="AC95">
+        <v>0</v>
+      </c>
+      <c r="AD95">
+        <v>0</v>
+      </c>
+      <c r="AE95">
+        <v>0</v>
+      </c>
+      <c r="AF95">
+        <v>0</v>
+      </c>
+      <c r="AG95">
+        <v>0</v>
+      </c>
+      <c r="AH95">
+        <v>0</v>
+      </c>
+      <c r="AI95">
+        <v>1</v>
+      </c>
+      <c r="AJ95">
+        <v>1</v>
+      </c>
+      <c r="AK95">
+        <v>1</v>
+      </c>
+      <c r="AL95">
+        <v>1</v>
+      </c>
+      <c r="AM95">
+        <v>1</v>
+      </c>
+      <c r="AN95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:40">
+      <c r="B96" t="s">
+        <v>139</v>
+      </c>
+      <c r="C96">
+        <v>30.3753</v>
+      </c>
+      <c r="D96">
+        <v>69.3451</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+      <c r="K96">
+        <v>0</v>
+      </c>
+      <c r="L96">
+        <v>0</v>
+      </c>
+      <c r="M96">
+        <v>0</v>
+      </c>
+      <c r="N96">
+        <v>0</v>
+      </c>
+      <c r="O96">
+        <v>0</v>
+      </c>
+      <c r="P96">
+        <v>0</v>
+      </c>
+      <c r="Q96">
+        <v>0</v>
+      </c>
+      <c r="R96">
+        <v>0</v>
+      </c>
+      <c r="S96">
+        <v>0</v>
+      </c>
+      <c r="T96">
+        <v>0</v>
+      </c>
+      <c r="U96">
+        <v>0</v>
+      </c>
+      <c r="V96">
+        <v>0</v>
+      </c>
+      <c r="W96">
+        <v>0</v>
+      </c>
+      <c r="X96">
+        <v>0</v>
+      </c>
+      <c r="Y96">
+        <v>0</v>
+      </c>
+      <c r="Z96">
+        <v>0</v>
+      </c>
+      <c r="AA96">
+        <v>0</v>
+      </c>
+      <c r="AB96">
+        <v>0</v>
+      </c>
+      <c r="AC96">
+        <v>0</v>
+      </c>
+      <c r="AD96">
+        <v>0</v>
+      </c>
+      <c r="AE96">
+        <v>0</v>
+      </c>
+      <c r="AF96">
+        <v>0</v>
+      </c>
+      <c r="AG96">
+        <v>0</v>
+      </c>
+      <c r="AH96">
+        <v>0</v>
+      </c>
+      <c r="AI96">
+        <v>0</v>
+      </c>
+      <c r="AJ96">
+        <v>0</v>
+      </c>
+      <c r="AK96">
+        <v>0</v>
+      </c>
+      <c r="AL96">
+        <v>0</v>
+      </c>
+      <c r="AM96">
+        <v>0</v>
+      </c>
+      <c r="AN96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="2:40">
+      <c r="B97" t="s">
+        <v>140</v>
+      </c>
+      <c r="C97">
+        <v>-14.235</v>
+      </c>
+      <c r="D97">
+        <v>-51.9253</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="L97">
+        <v>0</v>
+      </c>
+      <c r="M97">
+        <v>0</v>
+      </c>
+      <c r="N97">
+        <v>0</v>
+      </c>
+      <c r="O97">
+        <v>0</v>
+      </c>
+      <c r="P97">
+        <v>0</v>
+      </c>
+      <c r="Q97">
+        <v>0</v>
+      </c>
+      <c r="R97">
+        <v>0</v>
+      </c>
+      <c r="S97">
+        <v>0</v>
+      </c>
+      <c r="T97">
+        <v>0</v>
+      </c>
+      <c r="U97">
+        <v>0</v>
+      </c>
+      <c r="V97">
+        <v>0</v>
+      </c>
+      <c r="W97">
+        <v>0</v>
+      </c>
+      <c r="X97">
+        <v>0</v>
+      </c>
+      <c r="Y97">
+        <v>0</v>
+      </c>
+      <c r="Z97">
+        <v>0</v>
+      </c>
+      <c r="AA97">
+        <v>0</v>
+      </c>
+      <c r="AB97">
+        <v>0</v>
+      </c>
+      <c r="AC97">
+        <v>0</v>
+      </c>
+      <c r="AD97">
+        <v>0</v>
+      </c>
+      <c r="AE97">
+        <v>0</v>
+      </c>
+      <c r="AF97">
+        <v>0</v>
+      </c>
+      <c r="AG97">
+        <v>0</v>
+      </c>
+      <c r="AH97">
+        <v>0</v>
+      </c>
+      <c r="AI97">
+        <v>0</v>
+      </c>
+      <c r="AJ97">
+        <v>0</v>
+      </c>
+      <c r="AK97">
+        <v>0</v>
+      </c>
+      <c r="AL97">
+        <v>0</v>
+      </c>
+      <c r="AM97">
+        <v>0</v>
+      </c>
+      <c r="AN97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="2:40">
+      <c r="B98" t="s">
+        <v>141</v>
+      </c>
+      <c r="C98">
+        <v>42.3154</v>
+      </c>
+      <c r="D98">
+        <v>43.3569</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98">
+        <v>0</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+      <c r="K98">
+        <v>0</v>
+      </c>
+      <c r="L98">
+        <v>0</v>
+      </c>
+      <c r="M98">
+        <v>0</v>
+      </c>
+      <c r="N98">
+        <v>0</v>
+      </c>
+      <c r="O98">
+        <v>0</v>
+      </c>
+      <c r="P98">
+        <v>0</v>
+      </c>
+      <c r="Q98">
+        <v>0</v>
+      </c>
+      <c r="R98">
+        <v>0</v>
+      </c>
+      <c r="S98">
+        <v>0</v>
+      </c>
+      <c r="T98">
+        <v>0</v>
+      </c>
+      <c r="U98">
+        <v>0</v>
+      </c>
+      <c r="V98">
+        <v>0</v>
+      </c>
+      <c r="W98">
+        <v>0</v>
+      </c>
+      <c r="X98">
+        <v>0</v>
+      </c>
+      <c r="Y98">
+        <v>0</v>
+      </c>
+      <c r="Z98">
+        <v>0</v>
+      </c>
+      <c r="AA98">
+        <v>0</v>
+      </c>
+      <c r="AB98">
+        <v>0</v>
+      </c>
+      <c r="AC98">
+        <v>0</v>
+      </c>
+      <c r="AD98">
+        <v>0</v>
+      </c>
+      <c r="AE98">
+        <v>0</v>
+      </c>
+      <c r="AF98">
+        <v>0</v>
+      </c>
+      <c r="AG98">
+        <v>0</v>
+      </c>
+      <c r="AH98">
+        <v>0</v>
+      </c>
+      <c r="AI98">
+        <v>0</v>
+      </c>
+      <c r="AJ98">
+        <v>0</v>
+      </c>
+      <c r="AK98">
+        <v>0</v>
+      </c>
+      <c r="AL98">
+        <v>0</v>
+      </c>
+      <c r="AM98">
+        <v>0</v>
+      </c>
+      <c r="AN98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="2:40">
+      <c r="B99" t="s">
+        <v>142</v>
+      </c>
+      <c r="C99">
+        <v>39.0742</v>
+      </c>
+      <c r="D99">
+        <v>21.8243</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99">
+        <v>0</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+      <c r="K99">
+        <v>0</v>
+      </c>
+      <c r="L99">
+        <v>0</v>
+      </c>
+      <c r="M99">
+        <v>0</v>
+      </c>
+      <c r="N99">
+        <v>0</v>
+      </c>
+      <c r="O99">
+        <v>0</v>
+      </c>
+      <c r="P99">
+        <v>0</v>
+      </c>
+      <c r="Q99">
+        <v>0</v>
+      </c>
+      <c r="R99">
+        <v>0</v>
+      </c>
+      <c r="S99">
+        <v>0</v>
+      </c>
+      <c r="T99">
+        <v>0</v>
+      </c>
+      <c r="U99">
+        <v>0</v>
+      </c>
+      <c r="V99">
+        <v>0</v>
+      </c>
+      <c r="W99">
+        <v>0</v>
+      </c>
+      <c r="X99">
+        <v>0</v>
+      </c>
+      <c r="Y99">
+        <v>0</v>
+      </c>
+      <c r="Z99">
+        <v>0</v>
+      </c>
+      <c r="AA99">
+        <v>0</v>
+      </c>
+      <c r="AB99">
+        <v>0</v>
+      </c>
+      <c r="AC99">
+        <v>0</v>
+      </c>
+      <c r="AD99">
+        <v>0</v>
+      </c>
+      <c r="AE99">
+        <v>0</v>
+      </c>
+      <c r="AF99">
+        <v>0</v>
+      </c>
+      <c r="AG99">
+        <v>0</v>
+      </c>
+      <c r="AH99">
+        <v>0</v>
+      </c>
+      <c r="AI99">
+        <v>0</v>
+      </c>
+      <c r="AJ99">
+        <v>0</v>
+      </c>
+      <c r="AK99">
+        <v>0</v>
+      </c>
+      <c r="AL99">
+        <v>0</v>
+      </c>
+      <c r="AM99">
+        <v>0</v>
+      </c>
+      <c r="AN99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="2:40">
+      <c r="B100" t="s">
+        <v>143</v>
+      </c>
+      <c r="C100">
+        <v>41.6086</v>
+      </c>
+      <c r="D100">
+        <v>21.7453</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+      <c r="K100">
+        <v>0</v>
+      </c>
+      <c r="L100">
+        <v>0</v>
+      </c>
+      <c r="M100">
+        <v>0</v>
+      </c>
+      <c r="N100">
+        <v>0</v>
+      </c>
+      <c r="O100">
+        <v>0</v>
+      </c>
+      <c r="P100">
+        <v>0</v>
+      </c>
+      <c r="Q100">
+        <v>0</v>
+      </c>
+      <c r="R100">
+        <v>0</v>
+      </c>
+      <c r="S100">
+        <v>0</v>
+      </c>
+      <c r="T100">
+        <v>0</v>
+      </c>
+      <c r="U100">
+        <v>0</v>
+      </c>
+      <c r="V100">
+        <v>0</v>
+      </c>
+      <c r="W100">
+        <v>0</v>
+      </c>
+      <c r="X100">
+        <v>0</v>
+      </c>
+      <c r="Y100">
+        <v>0</v>
+      </c>
+      <c r="Z100">
+        <v>0</v>
+      </c>
+      <c r="AA100">
+        <v>0</v>
+      </c>
+      <c r="AB100">
+        <v>0</v>
+      </c>
+      <c r="AC100">
+        <v>0</v>
+      </c>
+      <c r="AD100">
+        <v>0</v>
+      </c>
+      <c r="AE100">
+        <v>0</v>
+      </c>
+      <c r="AF100">
+        <v>0</v>
+      </c>
+      <c r="AG100">
+        <v>0</v>
+      </c>
+      <c r="AH100">
+        <v>0</v>
+      </c>
+      <c r="AI100">
+        <v>0</v>
+      </c>
+      <c r="AJ100">
+        <v>0</v>
+      </c>
+      <c r="AK100">
+        <v>0</v>
+      </c>
+      <c r="AL100">
+        <v>0</v>
+      </c>
+      <c r="AM100">
+        <v>0</v>
+      </c>
+      <c r="AN100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="2:40">
+      <c r="B101" t="s">
+        <v>144</v>
+      </c>
+      <c r="C101">
+        <v>60.472</v>
+      </c>
+      <c r="D101">
+        <v>8.4689</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101">
+        <v>0</v>
+      </c>
+      <c r="J101">
+        <v>0</v>
+      </c>
+      <c r="K101">
+        <v>0</v>
+      </c>
+      <c r="L101">
+        <v>0</v>
+      </c>
+      <c r="M101">
+        <v>0</v>
+      </c>
+      <c r="N101">
+        <v>0</v>
+      </c>
+      <c r="O101">
+        <v>0</v>
+      </c>
+      <c r="P101">
+        <v>0</v>
+      </c>
+      <c r="Q101">
+        <v>0</v>
+      </c>
+      <c r="R101">
+        <v>0</v>
+      </c>
+      <c r="S101">
+        <v>0</v>
+      </c>
+      <c r="T101">
+        <v>0</v>
+      </c>
+      <c r="U101">
+        <v>0</v>
+      </c>
+      <c r="V101">
+        <v>0</v>
+      </c>
+      <c r="W101">
+        <v>0</v>
+      </c>
+      <c r="X101">
+        <v>0</v>
+      </c>
+      <c r="Y101">
+        <v>0</v>
+      </c>
+      <c r="Z101">
+        <v>0</v>
+      </c>
+      <c r="AA101">
+        <v>0</v>
+      </c>
+      <c r="AB101">
+        <v>0</v>
+      </c>
+      <c r="AC101">
+        <v>0</v>
+      </c>
+      <c r="AD101">
+        <v>0</v>
+      </c>
+      <c r="AE101">
+        <v>0</v>
+      </c>
+      <c r="AF101">
+        <v>0</v>
+      </c>
+      <c r="AG101">
+        <v>0</v>
+      </c>
+      <c r="AH101">
+        <v>0</v>
+      </c>
+      <c r="AI101">
+        <v>0</v>
+      </c>
+      <c r="AJ101">
+        <v>0</v>
+      </c>
+      <c r="AK101">
+        <v>0</v>
+      </c>
+      <c r="AL101">
+        <v>0</v>
+      </c>
+      <c r="AM101">
+        <v>0</v>
+      </c>
+      <c r="AN101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="2:40">
+      <c r="B102" t="s">
+        <v>145</v>
+      </c>
+      <c r="C102">
+        <v>45.9432</v>
+      </c>
+      <c r="D102">
+        <v>24.9668</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+      <c r="H102">
+        <v>0</v>
+      </c>
+      <c r="I102">
+        <v>0</v>
+      </c>
+      <c r="J102">
+        <v>0</v>
+      </c>
+      <c r="K102">
+        <v>0</v>
+      </c>
+      <c r="L102">
+        <v>0</v>
+      </c>
+      <c r="M102">
+        <v>0</v>
+      </c>
+      <c r="N102">
+        <v>0</v>
+      </c>
+      <c r="O102">
+        <v>0</v>
+      </c>
+      <c r="P102">
+        <v>0</v>
+      </c>
+      <c r="Q102">
+        <v>0</v>
+      </c>
+      <c r="R102">
+        <v>0</v>
+      </c>
+      <c r="S102">
+        <v>0</v>
+      </c>
+      <c r="T102">
+        <v>0</v>
+      </c>
+      <c r="U102">
+        <v>0</v>
+      </c>
+      <c r="V102">
+        <v>0</v>
+      </c>
+      <c r="W102">
+        <v>0</v>
+      </c>
+      <c r="X102">
+        <v>0</v>
+      </c>
+      <c r="Y102">
+        <v>0</v>
+      </c>
+      <c r="Z102">
+        <v>0</v>
+      </c>
+      <c r="AA102">
+        <v>0</v>
+      </c>
+      <c r="AB102">
+        <v>0</v>
+      </c>
+      <c r="AC102">
+        <v>0</v>
+      </c>
+      <c r="AD102">
+        <v>0</v>
+      </c>
+      <c r="AE102">
+        <v>0</v>
+      </c>
+      <c r="AF102">
+        <v>0</v>
+      </c>
+      <c r="AG102">
+        <v>0</v>
+      </c>
+      <c r="AH102">
+        <v>0</v>
+      </c>
+      <c r="AI102">
+        <v>0</v>
+      </c>
+      <c r="AJ102">
+        <v>0</v>
+      </c>
+      <c r="AK102">
+        <v>0</v>
+      </c>
+      <c r="AL102">
+        <v>0</v>
+      </c>
+      <c r="AM102">
+        <v>0</v>
+      </c>
+      <c r="AN102">
         <v>1</v>
       </c>
     </row>

</xml_diff>